<commit_message>
Primera prueba con formato, se añadio un json para configurar salida
</commit_message>
<xml_diff>
--- a/Himnos 2025 Abril.xlsx
+++ b/Himnos 2025 Abril.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\D'Aaron\Curso de Python\Hymn_List_Manager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\COMSITEC\Desktop\Aarón\Python Proyects\himn_list_manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -584,42 +584,6 @@
     <t>HIMNOS ABRIL 2025</t>
   </si>
   <si>
-    <t>MIERCOLES 2</t>
-  </si>
-  <si>
-    <t>DOMINGO  06 M</t>
-  </si>
-  <si>
-    <t>DOMINGO 06 T</t>
-  </si>
-  <si>
-    <t>DOMINGO 13 M</t>
-  </si>
-  <si>
-    <t>DOMINGO 13 T</t>
-  </si>
-  <si>
-    <t>DOMINGO 20 M</t>
-  </si>
-  <si>
-    <t>DOMINGO 20 T</t>
-  </si>
-  <si>
-    <t>DOMINGO 27 T</t>
-  </si>
-  <si>
-    <t>DOMINGO 27 M</t>
-  </si>
-  <si>
-    <t>MIERCOLES 09</t>
-  </si>
-  <si>
-    <t>MIERCOLES 16</t>
-  </si>
-  <si>
-    <t>MIERCOLES 23</t>
-  </si>
-  <si>
     <t>MIERCOLES 30</t>
   </si>
   <si>
@@ -690,6 +654,42 @@
   </si>
   <si>
     <t>Cantaré La Bella Historia</t>
+  </si>
+  <si>
+    <t>MIERCOLES 7</t>
+  </si>
+  <si>
+    <t>DOMINGO  11 M</t>
+  </si>
+  <si>
+    <t>DOMINGO 11 T</t>
+  </si>
+  <si>
+    <t>DOMINGO 18 M</t>
+  </si>
+  <si>
+    <t>DOMINGO 18 T</t>
+  </si>
+  <si>
+    <t>MIERCOLES 14</t>
+  </si>
+  <si>
+    <t>MIERCOLES 21</t>
+  </si>
+  <si>
+    <t>MIERCOLES 28</t>
+  </si>
+  <si>
+    <t>DOMINGO 25 M</t>
+  </si>
+  <si>
+    <t>DOMINGO 25 T</t>
+  </si>
+  <si>
+    <t>DOMINGO 1 M</t>
+  </si>
+  <si>
+    <t>DOMINGO 1 T</t>
   </si>
 </sst>
 </file>
@@ -2334,8 +2334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="U24" sqref="U23:U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2396,7 +2396,7 @@
       <c r="A2" s="259"/>
       <c r="B2" s="4"/>
       <c r="C2" s="20" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>2</v>
@@ -2410,7 +2410,7 @@
       <c r="G2" s="49"/>
       <c r="H2" s="4"/>
       <c r="I2" s="197" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>2</v>
@@ -2424,7 +2424,7 @@
       <c r="M2" s="49"/>
       <c r="N2" s="4"/>
       <c r="O2" s="109" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>2</v>
@@ -2704,7 +2704,7 @@
         <v>6</v>
       </c>
       <c r="I8" s="192" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="J8" s="156">
         <v>333</v>
@@ -2759,7 +2759,7 @@
       <c r="A10" s="259"/>
       <c r="B10" s="4"/>
       <c r="C10" s="20" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>2</v>
@@ -2773,7 +2773,7 @@
       <c r="G10" s="45"/>
       <c r="H10" s="2"/>
       <c r="I10" s="110" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>2</v>
@@ -2787,7 +2787,7 @@
       <c r="M10" s="49"/>
       <c r="N10" s="4"/>
       <c r="O10" s="109" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="P10" s="2" t="s">
         <v>2</v>
@@ -2816,7 +2816,7 @@
         <v>1</v>
       </c>
       <c r="I11" s="234" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="J11" s="246">
         <v>234</v>
@@ -2830,7 +2830,7 @@
         <v>1</v>
       </c>
       <c r="O11" s="234" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="P11" s="251">
         <v>39</v>
@@ -2922,7 +2922,7 @@
         <v>3</v>
       </c>
       <c r="O13" s="237" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="P13" s="156">
         <v>323</v>
@@ -2955,7 +2955,7 @@
         <v>4</v>
       </c>
       <c r="I14" s="234" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="J14" s="237" t="s">
         <v>33</v>
@@ -2971,7 +2971,7 @@
         <v>4</v>
       </c>
       <c r="O14" s="234" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="P14" s="211">
         <v>221</v>
@@ -3004,7 +3004,7 @@
         <v>5</v>
       </c>
       <c r="I15" s="237" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="J15" s="157">
         <v>330</v>
@@ -3065,7 +3065,7 @@
         <v>6</v>
       </c>
       <c r="O16" s="238" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="P16" s="191"/>
       <c r="Q16" s="156">
@@ -3112,7 +3112,7 @@
       <c r="A18" s="259"/>
       <c r="B18" s="4"/>
       <c r="C18" s="20" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>2</v>
@@ -3126,7 +3126,7 @@
       <c r="G18" s="49"/>
       <c r="H18" s="4"/>
       <c r="I18" s="109" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="J18" s="15" t="s">
         <v>2</v>
@@ -3140,7 +3140,7 @@
       <c r="M18" s="49"/>
       <c r="N18" s="4"/>
       <c r="O18" s="109" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="P18" s="2" t="s">
         <v>2</v>
@@ -3195,7 +3195,7 @@
         <v>1</v>
       </c>
       <c r="O19" s="245" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="P19" s="191">
         <v>3</v>
@@ -3220,7 +3220,7 @@
         <v>2</v>
       </c>
       <c r="C20" s="238" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="D20" s="157"/>
       <c r="E20" s="156">
@@ -3234,7 +3234,7 @@
         <v>2</v>
       </c>
       <c r="I20" s="234" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="J20" s="192" t="s">
         <v>33</v>
@@ -3287,7 +3287,7 @@
         <v>3</v>
       </c>
       <c r="I21" s="240" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="J21" s="242" t="s">
         <v>33</v>
@@ -3328,7 +3328,7 @@
         <v>4</v>
       </c>
       <c r="C22" s="240" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="D22" s="252">
         <v>126</v>
@@ -3454,7 +3454,7 @@
         <v>6</v>
       </c>
       <c r="I24" s="245" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="J24" s="156">
         <v>171</v>
@@ -3516,7 +3516,7 @@
       <c r="A26" s="259"/>
       <c r="B26" s="2"/>
       <c r="C26" s="136" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>2</v>
@@ -3530,7 +3530,7 @@
       <c r="G26" s="45"/>
       <c r="H26" s="4"/>
       <c r="I26" s="109" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>2</v>
@@ -3544,7 +3544,7 @@
       <c r="M26" s="49"/>
       <c r="N26" s="4"/>
       <c r="O26" s="109" t="s">
-        <v>108</v>
+        <v>136</v>
       </c>
       <c r="P26" s="2" t="s">
         <v>2</v>
@@ -3568,7 +3568,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="237" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="D27" s="156">
         <v>483</v>
@@ -3622,7 +3622,7 @@
         <v>2</v>
       </c>
       <c r="C28" s="237" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="D28" s="156">
         <v>377</v>
@@ -3678,7 +3678,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="208" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="D29" s="157">
         <v>452</v>
@@ -3734,7 +3734,7 @@
         <v>4</v>
       </c>
       <c r="C30" s="238" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="D30" s="156">
         <v>457</v>
@@ -3750,7 +3750,7 @@
         <v>4</v>
       </c>
       <c r="I30" s="223" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="J30" s="218" t="s">
         <v>33</v>
@@ -3790,7 +3790,7 @@
         <v>5</v>
       </c>
       <c r="C31" s="237" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="D31" s="156">
         <v>214</v>
@@ -3804,7 +3804,7 @@
         <v>5</v>
       </c>
       <c r="I31" s="224" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="J31" s="250">
         <v>118</v>
@@ -3874,7 +3874,7 @@
         <v>6</v>
       </c>
       <c r="O32" s="238" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="P32" s="156">
         <v>322</v>
@@ -3896,7 +3896,7 @@
       <c r="A34" s="260"/>
       <c r="B34" s="2"/>
       <c r="C34" s="136" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>2</v>
@@ -4010,7 +4010,7 @@
         <v>3</v>
       </c>
       <c r="C37" s="237" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="D37" s="156">
         <v>377</v>
@@ -4124,7 +4124,7 @@
         <v>6</v>
       </c>
       <c r="C40" s="192" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="D40" s="156">
         <v>144</v>

</xml_diff>

<commit_message>
Solucion de problema anterior, y mejora de presentacion y flujo en consola.
</commit_message>
<xml_diff>
--- a/Himnos 2025 Abril.xlsx
+++ b/Himnos 2025 Abril.xlsx
@@ -260,7 +260,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="144">
   <si>
     <t>Opcionales</t>
   </si>
@@ -690,6 +690,27 @@
   </si>
   <si>
     <t>DOMINGO 1 T</t>
+  </si>
+  <si>
+    <t>que todo el mundo cante al señor</t>
+  </si>
+  <si>
+    <t>suenen dulces himnos gratos al señor</t>
+  </si>
+  <si>
+    <t>cerca mas cerca</t>
+  </si>
+  <si>
+    <t>el vino a mi corazon</t>
+  </si>
+  <si>
+    <t>Jesús es mi rey soberano</t>
+  </si>
+  <si>
+    <t>regocijate en el</t>
+  </si>
+  <si>
+    <t>todas las promesas del señor</t>
   </si>
 </sst>
 </file>
@@ -921,7 +942,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1118,36 +1139,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FF8EAADB"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor rgb="FF8EAADB"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FF8EA9DB"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC5E0B3"/>
-        <bgColor rgb="FFC5E0B3"/>
       </patternFill>
     </fill>
   </fills>
@@ -1370,7 +1361,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="262">
+  <cellXfs count="276">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1780,7 +1771,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1788,7 +1778,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="23" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="23" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="20" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1854,24 +1843,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1884,27 +1861,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="29" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="31" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="32" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1915,83 +1875,11 @@
     <xf numFmtId="0" fontId="15" fillId="21" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="33" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="33" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="35" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="33" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="36" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="36" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="38" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2005,6 +1893,155 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2334,8 +2371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="U24" sqref="U23:U24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2365,25 +2402,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="257" t="s">
+      <c r="B1" s="208" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="258"/>
-      <c r="D1" s="258"/>
-      <c r="E1" s="258"/>
-      <c r="F1" s="258"/>
-      <c r="G1" s="258"/>
-      <c r="H1" s="258"/>
-      <c r="I1" s="258"/>
-      <c r="J1" s="258"/>
-      <c r="K1" s="258"/>
-      <c r="L1" s="258"/>
-      <c r="M1" s="258"/>
-      <c r="N1" s="258"/>
-      <c r="O1" s="258"/>
-      <c r="P1" s="258"/>
-      <c r="Q1" s="258"/>
-      <c r="R1" s="258"/>
+      <c r="C1" s="209"/>
+      <c r="D1" s="209"/>
+      <c r="E1" s="209"/>
+      <c r="F1" s="209"/>
+      <c r="G1" s="209"/>
+      <c r="H1" s="209"/>
+      <c r="I1" s="209"/>
+      <c r="J1" s="209"/>
+      <c r="K1" s="209"/>
+      <c r="L1" s="209"/>
+      <c r="M1" s="209"/>
+      <c r="N1" s="209"/>
+      <c r="O1" s="209"/>
+      <c r="P1" s="209"/>
+      <c r="Q1" s="209"/>
+      <c r="R1" s="209"/>
       <c r="S1" s="124"/>
       <c r="T1" s="124"/>
       <c r="U1" s="124"/>
@@ -2393,1765 +2430,1804 @@
       <c r="Y1" s="11"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="259"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="20" t="s">
+      <c r="A2" s="210"/>
+      <c r="B2" s="213"/>
+      <c r="C2" s="213" t="s">
         <v>125</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="214" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="88" t="s">
+      <c r="E2" s="215" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="214" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="49"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="197" t="s">
+      <c r="G2" s="216"/>
+      <c r="H2" s="213"/>
+      <c r="I2" s="217" t="s">
         <v>126</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="213" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="213" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="213" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="49"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="109" t="s">
+      <c r="M2" s="216"/>
+      <c r="N2" s="213"/>
+      <c r="O2" s="213" t="s">
         <v>127</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="214" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="214" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="214" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="45"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="49"/>
+      <c r="S2" s="218"/>
+      <c r="T2" s="216"/>
+      <c r="U2" s="216"/>
       <c r="V2" s="45"/>
       <c r="W2" s="45"/>
       <c r="X2" s="45"/>
       <c r="Y2" s="11"/>
     </row>
     <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="259"/>
-      <c r="B3" s="98">
+      <c r="A3" s="210"/>
+      <c r="B3" s="219">
         <v>1</v>
       </c>
-      <c r="C3" s="245" t="s">
+      <c r="C3" s="220" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="156">
+      <c r="D3" s="221">
         <v>22</v>
       </c>
-      <c r="E3" s="157"/>
-      <c r="F3" s="19">
+      <c r="E3" s="221"/>
+      <c r="F3" s="222">
         <v>90</v>
       </c>
-      <c r="G3" s="61"/>
-      <c r="H3" s="18">
+      <c r="G3" s="223"/>
+      <c r="H3" s="224">
         <v>1</v>
       </c>
-      <c r="I3" s="245" t="s">
+      <c r="I3" s="220" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="214">
+      <c r="J3" s="221">
         <v>33</v>
       </c>
-      <c r="K3" s="214">
+      <c r="K3" s="221">
         <v>1</v>
       </c>
-      <c r="L3" s="115">
+      <c r="L3" s="225">
         <v>107</v>
       </c>
-      <c r="M3" s="61"/>
-      <c r="N3" s="18">
+      <c r="M3" s="223"/>
+      <c r="N3" s="224">
         <v>1</v>
       </c>
-      <c r="O3" s="206"/>
-      <c r="P3" s="157"/>
-      <c r="Q3" s="156"/>
-      <c r="R3" s="22"/>
-      <c r="S3" s="44"/>
-      <c r="T3" s="50"/>
-      <c r="U3" s="68"/>
+      <c r="O3" s="220"/>
+      <c r="P3" s="221"/>
+      <c r="Q3" s="221"/>
+      <c r="R3" s="222"/>
+      <c r="S3" s="226"/>
+      <c r="T3" s="227"/>
+      <c r="U3" s="228"/>
       <c r="V3" s="82"/>
       <c r="W3" s="82"/>
       <c r="X3" s="46"/>
       <c r="Y3" s="13"/>
     </row>
     <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="259"/>
-      <c r="B4" s="18">
+      <c r="A4" s="210"/>
+      <c r="B4" s="224">
         <v>2</v>
       </c>
-      <c r="C4" s="238" t="s">
+      <c r="C4" s="220" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="156">
+      <c r="D4" s="221">
         <v>222</v>
       </c>
-      <c r="E4" s="157"/>
-      <c r="F4" s="34">
+      <c r="E4" s="221"/>
+      <c r="F4" s="229">
         <v>30</v>
       </c>
-      <c r="G4" s="61"/>
-      <c r="H4" s="18">
+      <c r="G4" s="223"/>
+      <c r="H4" s="224">
         <v>2</v>
       </c>
-      <c r="I4" s="208" t="s">
+      <c r="I4" s="230" t="s">
         <v>57</v>
       </c>
-      <c r="J4" s="249">
+      <c r="J4" s="231">
         <v>26</v>
       </c>
-      <c r="K4" s="157">
+      <c r="K4" s="221">
         <v>121</v>
       </c>
-      <c r="L4" s="21">
+      <c r="L4" s="232">
         <v>114</v>
       </c>
-      <c r="M4" s="61"/>
-      <c r="N4" s="18">
+      <c r="M4" s="223"/>
+      <c r="N4" s="224">
         <v>2</v>
       </c>
-      <c r="O4" s="158"/>
-      <c r="P4" s="156"/>
-      <c r="Q4" s="157"/>
-      <c r="R4" s="115"/>
-      <c r="S4" s="61"/>
-      <c r="T4" s="50"/>
-      <c r="U4" s="125"/>
+      <c r="O4" s="220"/>
+      <c r="P4" s="221"/>
+      <c r="Q4" s="221"/>
+      <c r="R4" s="225"/>
+      <c r="S4" s="223"/>
+      <c r="T4" s="227"/>
+      <c r="U4" s="233"/>
       <c r="V4" s="82"/>
       <c r="W4" s="55"/>
       <c r="X4" s="126"/>
       <c r="Y4" s="13"/>
     </row>
     <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="259"/>
-      <c r="B5" s="19">
+      <c r="A5" s="210"/>
+      <c r="B5" s="222">
         <v>3</v>
       </c>
-      <c r="C5" s="247" t="s">
+      <c r="C5" s="234" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="248">
+      <c r="D5" s="231">
         <v>154</v>
       </c>
-      <c r="E5" s="239">
+      <c r="E5" s="221">
         <v>162</v>
       </c>
-      <c r="F5" s="34">
+      <c r="F5" s="229">
         <v>113</v>
       </c>
-      <c r="G5" s="61"/>
-      <c r="H5" s="19">
+      <c r="G5" s="223"/>
+      <c r="H5" s="222">
         <v>3</v>
       </c>
-      <c r="I5" s="237" t="s">
+      <c r="I5" s="230" t="s">
         <v>77</v>
       </c>
-      <c r="J5" s="157">
+      <c r="J5" s="221">
         <v>1</v>
       </c>
-      <c r="K5" s="156">
+      <c r="K5" s="221">
         <v>18</v>
       </c>
-      <c r="L5" s="21">
+      <c r="L5" s="232">
         <v>117</v>
       </c>
-      <c r="M5" s="61"/>
-      <c r="N5" s="19">
+      <c r="M5" s="223"/>
+      <c r="N5" s="222">
         <v>3</v>
       </c>
-      <c r="O5" s="228"/>
-      <c r="P5" s="229"/>
-      <c r="Q5" s="203"/>
-      <c r="R5" s="113"/>
-      <c r="S5" s="61"/>
-      <c r="T5" s="46"/>
-      <c r="U5" s="76"/>
+      <c r="O5" s="235"/>
+      <c r="P5" s="236"/>
+      <c r="Q5" s="237"/>
+      <c r="R5" s="225"/>
+      <c r="S5" s="223"/>
+      <c r="T5" s="238"/>
+      <c r="U5" s="239"/>
       <c r="V5" s="127"/>
       <c r="W5" s="128"/>
       <c r="X5" s="126"/>
       <c r="Y5" s="13"/>
     </row>
     <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="259"/>
-      <c r="B6" s="18">
+      <c r="A6" s="210"/>
+      <c r="B6" s="224">
         <v>4</v>
       </c>
-      <c r="C6" s="234" t="s">
+      <c r="C6" s="240" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="156">
+      <c r="D6" s="221">
         <v>142</v>
       </c>
-      <c r="E6" s="244">
+      <c r="E6" s="241">
         <v>45</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="222">
         <v>127</v>
       </c>
-      <c r="G6" s="61"/>
-      <c r="H6" s="18">
+      <c r="G6" s="223"/>
+      <c r="H6" s="224">
         <v>4</v>
       </c>
-      <c r="I6" s="240" t="s">
+      <c r="I6" s="242" t="s">
         <v>99</v>
       </c>
-      <c r="J6" s="241">
+      <c r="J6" s="236">
         <v>328</v>
       </c>
-      <c r="K6" s="242" t="s">
+      <c r="K6" s="237" t="s">
         <v>33</v>
       </c>
-      <c r="L6" s="243">
+      <c r="L6" s="224">
         <v>144</v>
       </c>
-      <c r="M6" s="61"/>
-      <c r="N6" s="18">
+      <c r="M6" s="223"/>
+      <c r="N6" s="224">
         <v>4</v>
       </c>
-      <c r="O6" s="230"/>
-      <c r="P6" s="192"/>
-      <c r="Q6" s="192"/>
-      <c r="R6" s="22"/>
-      <c r="S6" s="61"/>
-      <c r="T6" s="50"/>
-      <c r="U6" s="76"/>
+      <c r="O6" s="234"/>
+      <c r="P6" s="220"/>
+      <c r="Q6" s="220"/>
+      <c r="R6" s="222"/>
+      <c r="S6" s="223"/>
+      <c r="T6" s="227"/>
+      <c r="U6" s="239"/>
       <c r="V6" s="129"/>
       <c r="W6" s="129"/>
       <c r="X6" s="82"/>
       <c r="Y6" s="13"/>
     </row>
     <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="259"/>
-      <c r="B7" s="19">
+      <c r="A7" s="210"/>
+      <c r="B7" s="222">
         <v>5</v>
       </c>
-      <c r="C7" s="192" t="s">
+      <c r="C7" s="220" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="156">
+      <c r="D7" s="221">
         <v>100</v>
       </c>
-      <c r="E7" s="157"/>
-      <c r="F7" s="22">
+      <c r="E7" s="221"/>
+      <c r="F7" s="222">
         <v>103</v>
       </c>
-      <c r="G7" s="61"/>
-      <c r="H7" s="22">
+      <c r="G7" s="223"/>
+      <c r="H7" s="222">
         <v>5</v>
       </c>
-      <c r="I7" s="234" t="s">
+      <c r="I7" s="240" t="s">
         <v>96</v>
       </c>
-      <c r="J7" s="192" t="s">
+      <c r="J7" s="220" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="192" t="s">
+      <c r="K7" s="220" t="s">
         <v>33</v>
       </c>
-      <c r="L7" s="34">
+      <c r="L7" s="229">
         <v>137</v>
       </c>
-      <c r="M7" s="61"/>
-      <c r="N7" s="19">
+      <c r="M7" s="223"/>
+      <c r="N7" s="222">
         <v>5</v>
       </c>
-      <c r="O7" s="192"/>
-      <c r="P7" s="156"/>
-      <c r="Q7" s="157"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="61"/>
-      <c r="T7" s="46"/>
-      <c r="U7" s="12"/>
+      <c r="O7" s="220"/>
+      <c r="P7" s="221"/>
+      <c r="Q7" s="221"/>
+      <c r="R7" s="232"/>
+      <c r="S7" s="223"/>
+      <c r="T7" s="238"/>
+      <c r="U7" s="243"/>
       <c r="V7" s="69"/>
       <c r="W7" s="69"/>
       <c r="X7" s="69"/>
       <c r="Y7" s="13"/>
     </row>
     <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="259"/>
-      <c r="B8" s="10">
+      <c r="A8" s="210"/>
+      <c r="B8" s="244">
         <v>6</v>
       </c>
-      <c r="C8" s="237" t="s">
+      <c r="C8" s="230" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="246">
+      <c r="D8" s="221">
         <v>157</v>
       </c>
-      <c r="E8" s="239">
+      <c r="E8" s="221">
         <v>60</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="224">
         <v>74</v>
       </c>
-      <c r="G8" s="61"/>
-      <c r="H8" s="14">
+      <c r="G8" s="223"/>
+      <c r="H8" s="244">
         <v>6</v>
       </c>
-      <c r="I8" s="192" t="s">
+      <c r="I8" s="220" t="s">
         <v>102</v>
       </c>
-      <c r="J8" s="156">
+      <c r="J8" s="221">
         <v>333</v>
       </c>
-      <c r="K8" s="157"/>
-      <c r="L8" s="207">
+      <c r="K8" s="221"/>
+      <c r="L8" s="244">
         <v>89</v>
       </c>
-      <c r="M8" s="61"/>
-      <c r="N8" s="10">
+      <c r="M8" s="223"/>
+      <c r="N8" s="244">
         <v>6</v>
       </c>
-      <c r="O8" s="192"/>
-      <c r="P8" s="156"/>
-      <c r="Q8" s="157"/>
-      <c r="R8" s="22"/>
-      <c r="S8" s="61"/>
-      <c r="T8" s="47"/>
-      <c r="U8" s="83"/>
+      <c r="O8" s="220"/>
+      <c r="P8" s="221"/>
+      <c r="Q8" s="221"/>
+      <c r="R8" s="222"/>
+      <c r="S8" s="223"/>
+      <c r="T8" s="245"/>
+      <c r="U8" s="246"/>
       <c r="V8" s="51"/>
       <c r="W8" s="52"/>
       <c r="X8" s="70"/>
       <c r="Y8" s="13"/>
     </row>
     <row r="9" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="261"/>
-      <c r="C9" s="261"/>
-      <c r="D9" s="261"/>
-      <c r="E9" s="261"/>
-      <c r="F9" s="261"/>
-      <c r="G9" s="261"/>
-      <c r="H9" s="261"/>
-      <c r="I9" s="261"/>
-      <c r="J9" s="261"/>
-      <c r="K9" s="261"/>
-      <c r="L9" s="261"/>
-      <c r="M9" s="261"/>
-      <c r="N9" s="261"/>
-      <c r="O9" s="261"/>
-      <c r="P9" s="261"/>
-      <c r="Q9" s="261"/>
-      <c r="R9" s="261"/>
-      <c r="S9" s="261"/>
-      <c r="T9" s="261"/>
-      <c r="U9" s="261"/>
+      <c r="B9" s="247"/>
+      <c r="C9" s="247"/>
+      <c r="D9" s="247"/>
+      <c r="E9" s="247"/>
+      <c r="F9" s="247"/>
+      <c r="G9" s="247"/>
+      <c r="H9" s="247"/>
+      <c r="I9" s="247"/>
+      <c r="J9" s="247"/>
+      <c r="K9" s="247"/>
+      <c r="L9" s="247"/>
+      <c r="M9" s="247"/>
+      <c r="N9" s="247"/>
+      <c r="O9" s="247"/>
+      <c r="P9" s="247"/>
+      <c r="Q9" s="247"/>
+      <c r="R9" s="247"/>
+      <c r="S9" s="247"/>
+      <c r="T9" s="247"/>
+      <c r="U9" s="247"/>
       <c r="V9" s="5"/>
       <c r="W9" s="5"/>
       <c r="X9" s="5"/>
       <c r="Y9" s="11"/>
     </row>
     <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="259"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="20" t="s">
+      <c r="A10" s="210"/>
+      <c r="B10" s="213"/>
+      <c r="C10" s="213" t="s">
         <v>130</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="214" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="214" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="214" t="s">
         <v>1</v>
       </c>
-      <c r="G10" s="45"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="110" t="s">
+      <c r="G10" s="218"/>
+      <c r="H10" s="214"/>
+      <c r="I10" s="214" t="s">
         <v>128</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="214" t="s">
         <v>2</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="214" t="s">
         <v>3</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="L10" s="214" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="49"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="109" t="s">
+      <c r="M10" s="216"/>
+      <c r="N10" s="213"/>
+      <c r="O10" s="213" t="s">
         <v>129</v>
       </c>
-      <c r="P10" s="2" t="s">
+      <c r="P10" s="214" t="s">
         <v>2</v>
       </c>
-      <c r="Q10" s="2" t="s">
+      <c r="Q10" s="214" t="s">
         <v>3</v>
       </c>
-      <c r="R10" s="2" t="s">
+      <c r="R10" s="214" t="s">
         <v>1</v>
       </c>
-      <c r="S10" s="49"/>
-      <c r="T10" s="49"/>
+      <c r="S10" s="216"/>
+      <c r="T10" s="216"/>
+      <c r="U10" s="243"/>
       <c r="Y10" s="11"/>
     </row>
     <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="259"/>
-      <c r="B11" s="18">
+      <c r="A11" s="210"/>
+      <c r="B11" s="224">
         <v>1</v>
       </c>
-      <c r="C11" s="226"/>
-      <c r="D11" s="212"/>
-      <c r="E11" s="218"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="18">
+      <c r="C11" s="230"/>
+      <c r="D11" s="248"/>
+      <c r="E11" s="248"/>
+      <c r="F11" s="224"/>
+      <c r="G11" s="223"/>
+      <c r="H11" s="224">
         <v>1</v>
       </c>
-      <c r="I11" s="234" t="s">
+      <c r="I11" s="240" t="s">
         <v>104</v>
       </c>
-      <c r="J11" s="246">
+      <c r="J11" s="221">
         <v>234</v>
       </c>
-      <c r="K11" s="238"/>
-      <c r="L11" s="21">
+      <c r="K11" s="220"/>
+      <c r="L11" s="232">
         <v>128</v>
       </c>
-      <c r="M11" s="61"/>
-      <c r="N11" s="18">
+      <c r="M11" s="223"/>
+      <c r="N11" s="224">
         <v>1</v>
       </c>
-      <c r="O11" s="234" t="s">
+      <c r="O11" s="240" t="s">
         <v>110</v>
       </c>
-      <c r="P11" s="251">
+      <c r="P11" s="248">
         <v>39</v>
       </c>
-      <c r="Q11" s="237"/>
-      <c r="R11" s="99">
+      <c r="Q11" s="230"/>
+      <c r="R11" s="249">
         <v>130</v>
       </c>
-      <c r="S11" s="61"/>
-      <c r="T11" s="50"/>
-      <c r="U11" s="76"/>
+      <c r="S11" s="223"/>
+      <c r="T11" s="227"/>
+      <c r="U11" s="239"/>
       <c r="V11" s="130"/>
       <c r="W11" s="127"/>
       <c r="X11" s="82"/>
       <c r="Y11" s="11"/>
     </row>
     <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="259"/>
-      <c r="B12" s="18">
+      <c r="A12" s="210"/>
+      <c r="B12" s="224">
         <v>2</v>
       </c>
-      <c r="C12" s="208"/>
-      <c r="D12" s="231"/>
-      <c r="E12" s="222"/>
-      <c r="F12" s="118"/>
-      <c r="G12" s="61"/>
-      <c r="H12" s="18">
+      <c r="C12" s="230"/>
+      <c r="D12" s="250"/>
+      <c r="E12" s="251"/>
+      <c r="F12" s="252"/>
+      <c r="G12" s="223"/>
+      <c r="H12" s="224">
         <v>2</v>
       </c>
-      <c r="I12" s="208" t="s">
+      <c r="I12" s="230" t="s">
         <v>92</v>
       </c>
-      <c r="J12" s="212">
+      <c r="J12" s="248">
         <v>53</v>
       </c>
-      <c r="K12" s="218"/>
-      <c r="L12" s="113">
+      <c r="K12" s="248"/>
+      <c r="L12" s="225">
         <v>125</v>
       </c>
-      <c r="M12" s="61"/>
-      <c r="N12" s="18">
+      <c r="M12" s="223"/>
+      <c r="N12" s="224">
         <v>2</v>
       </c>
-      <c r="O12" s="237" t="s">
+      <c r="O12" s="230" t="s">
         <v>86</v>
       </c>
-      <c r="P12" s="157"/>
-      <c r="Q12" s="156">
+      <c r="P12" s="221"/>
+      <c r="Q12" s="221">
         <v>221</v>
       </c>
-      <c r="R12" s="34">
+      <c r="R12" s="229">
         <v>108</v>
       </c>
-      <c r="S12" s="61"/>
-      <c r="T12" s="50"/>
-      <c r="U12" s="131"/>
+      <c r="S12" s="223"/>
+      <c r="T12" s="227"/>
+      <c r="U12" s="253"/>
       <c r="V12" s="132"/>
       <c r="W12" s="133"/>
       <c r="X12" s="82"/>
       <c r="Y12" s="11"/>
     </row>
     <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="259"/>
-      <c r="B13" s="115">
+      <c r="A13" s="210"/>
+      <c r="B13" s="225">
         <v>3</v>
       </c>
-      <c r="C13" s="226"/>
-      <c r="D13" s="222"/>
-      <c r="E13" s="210"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="19">
+      <c r="C13" s="230"/>
+      <c r="D13" s="251"/>
+      <c r="E13" s="251"/>
+      <c r="F13" s="224"/>
+      <c r="G13" s="223"/>
+      <c r="H13" s="222">
         <v>3</v>
       </c>
-      <c r="I13" s="237" t="s">
+      <c r="I13" s="230" t="s">
         <v>93</v>
       </c>
-      <c r="J13" s="157">
+      <c r="J13" s="221">
         <v>98</v>
       </c>
-      <c r="K13" s="156">
+      <c r="K13" s="221">
         <v>56</v>
       </c>
-      <c r="L13" s="25">
+      <c r="L13" s="254">
         <v>65</v>
       </c>
-      <c r="M13" s="61"/>
-      <c r="N13" s="19">
+      <c r="M13" s="223"/>
+      <c r="N13" s="222">
         <v>3</v>
       </c>
-      <c r="O13" s="237" t="s">
+      <c r="O13" s="230" t="s">
         <v>112</v>
       </c>
-      <c r="P13" s="156">
+      <c r="P13" s="221">
         <v>323</v>
       </c>
-      <c r="Q13" s="157">
+      <c r="Q13" s="221">
         <v>123</v>
       </c>
-      <c r="R13" s="25">
+      <c r="R13" s="254">
         <v>111</v>
       </c>
-      <c r="S13" s="61"/>
-      <c r="T13" s="46"/>
-      <c r="U13" s="134"/>
+      <c r="S13" s="223"/>
+      <c r="T13" s="238"/>
+      <c r="U13" s="255"/>
       <c r="V13" s="130"/>
-      <c r="W13" s="225"/>
+      <c r="W13" s="206"/>
       <c r="X13" s="82"/>
       <c r="Y13" s="11"/>
     </row>
     <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="259"/>
-      <c r="B14" s="18">
+      <c r="A14" s="210"/>
+      <c r="B14" s="224">
         <v>4</v>
       </c>
-      <c r="C14" s="223"/>
-      <c r="D14" s="219"/>
-      <c r="E14" s="220"/>
-      <c r="F14" s="115"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="18">
+      <c r="C14" s="242"/>
+      <c r="D14" s="256"/>
+      <c r="E14" s="257"/>
+      <c r="F14" s="225"/>
+      <c r="G14" s="223"/>
+      <c r="H14" s="224">
         <v>4</v>
       </c>
-      <c r="I14" s="234" t="s">
+      <c r="I14" s="240" t="s">
         <v>109</v>
       </c>
-      <c r="J14" s="237" t="s">
+      <c r="J14" s="230" t="s">
         <v>33</v>
       </c>
-      <c r="K14" s="237" t="s">
+      <c r="K14" s="230" t="s">
         <v>33</v>
       </c>
-      <c r="L14" s="21">
+      <c r="L14" s="232">
         <v>132</v>
       </c>
-      <c r="M14" s="61"/>
-      <c r="N14" s="18">
+      <c r="M14" s="223"/>
+      <c r="N14" s="224">
         <v>4</v>
       </c>
-      <c r="O14" s="234" t="s">
+      <c r="O14" s="240" t="s">
         <v>105</v>
       </c>
-      <c r="P14" s="211">
+      <c r="P14" s="258">
         <v>221</v>
       </c>
-      <c r="Q14" s="213" t="s">
+      <c r="Q14" s="259" t="s">
         <v>33</v>
       </c>
-      <c r="R14" s="28">
+      <c r="R14" s="224">
         <v>141</v>
       </c>
-      <c r="S14" s="61"/>
-      <c r="T14" s="50"/>
-      <c r="U14" s="81"/>
+      <c r="S14" s="223"/>
+      <c r="T14" s="227"/>
+      <c r="U14" s="260"/>
       <c r="V14" s="127"/>
       <c r="W14" s="130"/>
       <c r="X14" s="46"/>
       <c r="Y14" s="11"/>
     </row>
     <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="259"/>
-      <c r="B15" s="19">
+      <c r="A15" s="210"/>
+      <c r="B15" s="222">
         <v>5</v>
       </c>
-      <c r="C15" s="221"/>
-      <c r="D15" s="210"/>
-      <c r="E15" s="210"/>
-      <c r="F15" s="113"/>
-      <c r="G15" s="61"/>
-      <c r="H15" s="22">
+      <c r="C15" s="261"/>
+      <c r="D15" s="251"/>
+      <c r="E15" s="251"/>
+      <c r="F15" s="225"/>
+      <c r="G15" s="223"/>
+      <c r="H15" s="222">
         <v>5</v>
       </c>
-      <c r="I15" s="237" t="s">
+      <c r="I15" s="230" t="s">
         <v>123</v>
       </c>
-      <c r="J15" s="157">
+      <c r="J15" s="221">
         <v>330</v>
       </c>
-      <c r="K15" s="156">
+      <c r="K15" s="221">
         <v>158</v>
       </c>
-      <c r="L15" s="99">
+      <c r="L15" s="249">
         <v>62</v>
       </c>
-      <c r="M15" s="61"/>
-      <c r="N15" s="19">
+      <c r="M15" s="223"/>
+      <c r="N15" s="222">
         <v>5</v>
       </c>
-      <c r="O15" s="192" t="s">
-        <v>16</v>
-      </c>
-      <c r="P15" s="156">
+      <c r="O15" s="207" t="s">
+        <v>139</v>
+      </c>
+      <c r="P15" s="221">
         <v>100</v>
       </c>
-      <c r="Q15" s="157"/>
-      <c r="R15" s="22">
+      <c r="Q15" s="221"/>
+      <c r="R15" s="222">
         <v>103</v>
       </c>
-      <c r="S15" s="61"/>
-      <c r="T15" s="46"/>
-      <c r="U15" s="131"/>
+      <c r="S15" s="223"/>
+      <c r="T15" s="238"/>
+      <c r="U15" s="253"/>
       <c r="V15" s="132"/>
       <c r="W15" s="135"/>
       <c r="X15" s="82"/>
       <c r="Y15" s="11"/>
     </row>
     <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="259"/>
-      <c r="B16" s="10">
+      <c r="A16" s="210"/>
+      <c r="B16" s="244">
         <v>6</v>
       </c>
-      <c r="C16" s="192"/>
-      <c r="D16" s="222"/>
-      <c r="E16" s="210"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="61"/>
-      <c r="H16" s="14">
+      <c r="C16" s="220"/>
+      <c r="D16" s="251"/>
+      <c r="E16" s="251"/>
+      <c r="F16" s="229"/>
+      <c r="G16" s="223"/>
+      <c r="H16" s="244">
         <v>6</v>
       </c>
-      <c r="I16" s="192" t="s">
+      <c r="I16" s="220" t="s">
         <v>28</v>
       </c>
-      <c r="J16" s="157"/>
-      <c r="K16" s="156">
+      <c r="J16" s="221"/>
+      <c r="K16" s="221">
         <v>278</v>
       </c>
-      <c r="L16" s="14">
+      <c r="L16" s="244">
         <v>109</v>
       </c>
-      <c r="M16" s="71"/>
-      <c r="N16" s="10">
+      <c r="M16" s="262"/>
+      <c r="N16" s="244">
         <v>6</v>
       </c>
-      <c r="O16" s="238" t="s">
+      <c r="O16" s="220" t="s">
         <v>113</v>
       </c>
-      <c r="P16" s="191"/>
-      <c r="Q16" s="156">
+      <c r="P16" s="221"/>
+      <c r="Q16" s="221">
         <v>131</v>
       </c>
-      <c r="R16" s="34">
+      <c r="R16" s="229">
         <v>41</v>
       </c>
-      <c r="S16" s="61"/>
-      <c r="T16" s="47"/>
-      <c r="U16" s="76"/>
+      <c r="S16" s="223"/>
+      <c r="T16" s="245"/>
+      <c r="U16" s="239"/>
       <c r="V16" s="130"/>
       <c r="W16" s="127"/>
       <c r="X16" s="46"/>
       <c r="Y16" s="11"/>
     </row>
     <row r="17" spans="1:25" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="11"/>
-      <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
+      <c r="B17" s="263"/>
+      <c r="C17" s="263"/>
+      <c r="D17" s="223"/>
+      <c r="E17" s="223"/>
+      <c r="F17" s="227"/>
+      <c r="G17" s="263"/>
+      <c r="H17" s="263"/>
+      <c r="I17" s="263"/>
+      <c r="J17" s="226"/>
+      <c r="K17" s="226"/>
+      <c r="L17" s="226"/>
+      <c r="M17" s="263"/>
+      <c r="N17" s="263"/>
+      <c r="O17" s="263"/>
+      <c r="P17" s="263"/>
+      <c r="Q17" s="263"/>
+      <c r="R17" s="263"/>
+      <c r="S17" s="263"/>
+      <c r="T17" s="263"/>
+      <c r="U17" s="263"/>
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
       <c r="Y17" s="11"/>
     </row>
     <row r="18" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="259"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="20" t="s">
+      <c r="A18" s="210"/>
+      <c r="B18" s="213"/>
+      <c r="C18" s="213" t="s">
         <v>131</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="213" t="s">
         <v>2</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="264" t="s">
         <v>3</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="213" t="s">
         <v>1</v>
       </c>
-      <c r="G18" s="49"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="109" t="s">
+      <c r="G18" s="216"/>
+      <c r="H18" s="213"/>
+      <c r="I18" s="213" t="s">
         <v>133</v>
       </c>
-      <c r="J18" s="15" t="s">
+      <c r="J18" s="265" t="s">
         <v>2</v>
       </c>
-      <c r="K18" s="88" t="s">
+      <c r="K18" s="215" t="s">
         <v>3</v>
       </c>
-      <c r="L18" s="2" t="s">
+      <c r="L18" s="214" t="s">
         <v>1</v>
       </c>
-      <c r="M18" s="49"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="109" t="s">
+      <c r="M18" s="216"/>
+      <c r="N18" s="213"/>
+      <c r="O18" s="213" t="s">
         <v>134</v>
       </c>
-      <c r="P18" s="2" t="s">
+      <c r="P18" s="214" t="s">
         <v>2</v>
       </c>
-      <c r="Q18" s="2" t="s">
+      <c r="Q18" s="214" t="s">
         <v>3</v>
       </c>
-      <c r="R18" s="2" t="s">
+      <c r="R18" s="214" t="s">
         <v>1</v>
       </c>
-      <c r="S18" s="45"/>
-      <c r="T18" s="45"/>
-      <c r="U18" s="45"/>
+      <c r="S18" s="218"/>
+      <c r="T18" s="218"/>
+      <c r="U18" s="218"/>
       <c r="V18" s="45"/>
       <c r="W18" s="45"/>
       <c r="X18" s="45"/>
       <c r="Y18"/>
     </row>
     <row r="19" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="259"/>
-      <c r="B19" s="18">
+      <c r="A19" s="210"/>
+      <c r="B19" s="224">
         <v>1</v>
       </c>
-      <c r="C19" s="237" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="156">
+      <c r="C19" s="205" t="s">
+        <v>137</v>
+      </c>
+      <c r="D19" s="221">
         <v>397</v>
       </c>
-      <c r="E19" s="157">
+      <c r="E19" s="221">
         <v>165</v>
       </c>
-      <c r="F19" s="34">
+      <c r="F19" s="229">
         <v>61</v>
       </c>
-      <c r="G19" s="61"/>
-      <c r="H19" s="18">
+      <c r="G19" s="223"/>
+      <c r="H19" s="224">
         <v>1</v>
       </c>
-      <c r="I19" s="237" t="s">
+      <c r="I19" s="230" t="s">
         <v>72</v>
       </c>
-      <c r="J19" s="239">
+      <c r="J19" s="221">
         <v>466</v>
       </c>
-      <c r="K19" s="246"/>
-      <c r="L19" s="22">
+      <c r="K19" s="221"/>
+      <c r="L19" s="222">
         <v>53</v>
       </c>
-      <c r="M19" s="61"/>
-      <c r="N19" s="18">
+      <c r="M19" s="223"/>
+      <c r="N19" s="224">
         <v>1</v>
       </c>
-      <c r="O19" s="245" t="s">
+      <c r="O19" s="220" t="s">
         <v>121</v>
       </c>
-      <c r="P19" s="191">
+      <c r="P19" s="221">
         <v>3</v>
       </c>
-      <c r="Q19" s="156">
+      <c r="Q19" s="221">
         <v>5</v>
       </c>
-      <c r="R19" s="22">
+      <c r="R19" s="222">
         <v>14</v>
       </c>
-      <c r="S19" s="44"/>
-      <c r="T19" s="50"/>
-      <c r="U19" s="56"/>
+      <c r="S19" s="226"/>
+      <c r="T19" s="227"/>
+      <c r="U19" s="266"/>
       <c r="V19" s="57"/>
       <c r="W19" s="58"/>
       <c r="X19" s="59"/>
       <c r="Y19"/>
     </row>
     <row r="20" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="259"/>
-      <c r="B20" s="18">
+      <c r="A20" s="210"/>
+      <c r="B20" s="224">
         <v>2</v>
       </c>
-      <c r="C20" s="238" t="s">
+      <c r="C20" s="220" t="s">
         <v>116</v>
       </c>
-      <c r="D20" s="157"/>
-      <c r="E20" s="156">
+      <c r="D20" s="221"/>
+      <c r="E20" s="221">
         <v>207</v>
       </c>
-      <c r="F20" s="207">
+      <c r="F20" s="244">
         <v>59</v>
       </c>
-      <c r="G20" s="61"/>
-      <c r="H20" s="18">
+      <c r="G20" s="223"/>
+      <c r="H20" s="224">
         <v>2</v>
       </c>
-      <c r="I20" s="234" t="s">
+      <c r="I20" s="240" t="s">
         <v>103</v>
       </c>
-      <c r="J20" s="192" t="s">
+      <c r="J20" s="220" t="s">
         <v>33</v>
       </c>
-      <c r="K20" s="192" t="s">
+      <c r="K20" s="220" t="s">
         <v>33</v>
       </c>
-      <c r="L20" s="115">
+      <c r="L20" s="225">
         <v>138</v>
       </c>
-      <c r="M20" s="61"/>
-      <c r="N20" s="18">
+      <c r="M20" s="223"/>
+      <c r="N20" s="224">
         <v>2</v>
       </c>
-      <c r="O20" s="208" t="s">
+      <c r="O20" s="230" t="s">
         <v>30</v>
       </c>
-      <c r="P20" s="156">
+      <c r="P20" s="221">
         <v>460</v>
       </c>
-      <c r="Q20" s="191"/>
-      <c r="R20" s="22">
+      <c r="Q20" s="221"/>
+      <c r="R20" s="222">
         <v>7</v>
       </c>
-      <c r="S20" s="61"/>
-      <c r="T20" s="50"/>
-      <c r="U20" s="75"/>
+      <c r="S20" s="223"/>
+      <c r="T20" s="227"/>
+      <c r="U20" s="267"/>
       <c r="V20" s="75"/>
       <c r="W20" s="75"/>
       <c r="X20" s="59"/>
       <c r="Y20"/>
     </row>
     <row r="21" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="259"/>
-      <c r="B21" s="19">
+      <c r="A21" s="210"/>
+      <c r="B21" s="222">
         <v>3</v>
       </c>
-      <c r="C21" s="238" t="s">
+      <c r="C21" s="220" t="s">
         <v>63</v>
       </c>
-      <c r="D21" s="156">
+      <c r="D21" s="221">
         <v>218</v>
       </c>
-      <c r="E21" s="157"/>
-      <c r="F21" s="113">
+      <c r="E21" s="221"/>
+      <c r="F21" s="225">
         <v>63</v>
       </c>
-      <c r="G21" s="61"/>
-      <c r="H21" s="19">
+      <c r="G21" s="223"/>
+      <c r="H21" s="222">
         <v>3</v>
       </c>
-      <c r="I21" s="240" t="s">
+      <c r="I21" s="242" t="s">
         <v>106</v>
       </c>
-      <c r="J21" s="242" t="s">
+      <c r="J21" s="237" t="s">
         <v>33</v>
       </c>
-      <c r="K21" s="242" t="s">
+      <c r="K21" s="237" t="s">
         <v>33</v>
       </c>
-      <c r="L21" s="34">
+      <c r="L21" s="229">
         <v>145</v>
       </c>
-      <c r="M21" s="61"/>
-      <c r="N21" s="19">
+      <c r="M21" s="223"/>
+      <c r="N21" s="222">
         <v>3</v>
       </c>
-      <c r="O21" s="237" t="s">
+      <c r="O21" s="230" t="s">
         <v>49</v>
       </c>
-      <c r="P21" s="214">
+      <c r="P21" s="221">
         <v>110</v>
       </c>
-      <c r="Q21" s="214">
+      <c r="Q21" s="221">
         <v>59</v>
       </c>
-      <c r="R21" s="115">
+      <c r="R21" s="225">
         <v>122</v>
       </c>
-      <c r="S21" s="50"/>
-      <c r="T21" s="123"/>
-      <c r="U21" s="56"/>
+      <c r="S21" s="227"/>
+      <c r="T21" s="268"/>
+      <c r="U21" s="266"/>
       <c r="V21" s="51"/>
       <c r="W21" s="52"/>
       <c r="X21" s="44"/>
       <c r="Y21"/>
     </row>
     <row r="22" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="259"/>
-      <c r="B22" s="18">
+      <c r="A22" s="210"/>
+      <c r="B22" s="224">
         <v>4</v>
       </c>
-      <c r="C22" s="240" t="s">
+      <c r="C22" s="242" t="s">
         <v>111</v>
       </c>
-      <c r="D22" s="252">
+      <c r="D22" s="236">
         <v>126</v>
       </c>
-      <c r="E22" s="253" t="s">
+      <c r="E22" s="237" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="113">
+      <c r="F22" s="225">
         <v>146</v>
       </c>
-      <c r="G22" s="61"/>
-      <c r="H22" s="18">
+      <c r="G22" s="223"/>
+      <c r="H22" s="224">
         <v>4</v>
       </c>
-      <c r="I22" s="192" t="s">
+      <c r="I22" s="220" t="s">
         <v>60</v>
       </c>
-      <c r="J22" s="156">
+      <c r="J22" s="221">
         <v>125</v>
       </c>
-      <c r="K22" s="156">
+      <c r="K22" s="221">
         <v>47</v>
       </c>
-      <c r="L22" s="22">
+      <c r="L22" s="222">
         <v>98</v>
       </c>
-      <c r="M22" s="61"/>
-      <c r="N22" s="18">
+      <c r="M22" s="223"/>
+      <c r="N22" s="224">
         <v>4</v>
       </c>
-      <c r="O22" s="234" t="s">
-        <v>96</v>
-      </c>
-      <c r="P22" s="192" t="s">
+      <c r="O22" s="205" t="s">
+        <v>140</v>
+      </c>
+      <c r="P22" s="220" t="s">
         <v>33</v>
       </c>
-      <c r="Q22" s="192" t="s">
+      <c r="Q22" s="220" t="s">
         <v>33</v>
       </c>
-      <c r="R22" s="28">
+      <c r="R22" s="224">
         <v>137</v>
       </c>
-      <c r="S22" s="61"/>
-      <c r="T22" s="50"/>
-      <c r="U22" s="76"/>
+      <c r="S22" s="223"/>
+      <c r="T22" s="227"/>
+      <c r="U22" s="239"/>
       <c r="V22" s="77"/>
       <c r="W22" s="78"/>
       <c r="X22" s="44"/>
       <c r="Y22"/>
     </row>
     <row r="23" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="259"/>
-      <c r="B23" s="91">
+      <c r="A23" s="210"/>
+      <c r="B23" s="269">
         <v>5</v>
       </c>
-      <c r="C23" s="238" t="s">
+      <c r="C23" s="220" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="157">
+      <c r="D23" s="221">
         <v>484</v>
       </c>
-      <c r="E23" s="156">
+      <c r="E23" s="221">
         <v>116</v>
       </c>
-      <c r="F23" s="25">
+      <c r="F23" s="254">
         <v>49</v>
       </c>
-      <c r="G23" s="61"/>
-      <c r="H23" s="91">
+      <c r="G23" s="223"/>
+      <c r="H23" s="269">
         <v>5</v>
       </c>
-      <c r="I23" s="245" t="s">
+      <c r="I23" s="220" t="s">
         <v>11</v>
       </c>
-      <c r="J23" s="156">
+      <c r="J23" s="221">
         <v>20</v>
       </c>
-      <c r="K23" s="157"/>
-      <c r="L23" s="22">
+      <c r="K23" s="221"/>
+      <c r="L23" s="222">
         <v>48</v>
       </c>
-      <c r="M23" s="61"/>
-      <c r="N23" s="19">
+      <c r="M23" s="223"/>
+      <c r="N23" s="222">
         <v>5</v>
       </c>
-      <c r="O23" s="237" t="s">
+      <c r="O23" s="230" t="s">
         <v>23</v>
       </c>
-      <c r="P23" s="156">
+      <c r="P23" s="221">
         <v>183</v>
       </c>
-      <c r="Q23" s="157"/>
-      <c r="R23" s="22">
+      <c r="Q23" s="221"/>
+      <c r="R23" s="222">
         <v>112</v>
       </c>
-      <c r="S23" s="61"/>
-      <c r="T23" s="46"/>
-      <c r="U23" s="56"/>
+      <c r="S23" s="223"/>
+      <c r="T23" s="238"/>
+      <c r="U23" s="266"/>
       <c r="V23" s="57"/>
       <c r="W23" s="58"/>
       <c r="X23" s="59"/>
       <c r="Y23"/>
     </row>
     <row r="24" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="259"/>
-      <c r="B24" s="10">
+      <c r="A24" s="210"/>
+      <c r="B24" s="244">
         <v>6</v>
       </c>
-      <c r="C24" s="226" t="s">
+      <c r="C24" s="205" t="s">
+        <v>138</v>
+      </c>
+      <c r="D24" s="221">
+        <v>427</v>
+      </c>
+      <c r="E24" s="221">
+        <v>323</v>
+      </c>
+      <c r="F24" s="224">
+        <v>66</v>
+      </c>
+      <c r="G24" s="223"/>
+      <c r="H24" s="244">
+        <v>6</v>
+      </c>
+      <c r="I24" s="220" t="s">
+        <v>122</v>
+      </c>
+      <c r="J24" s="221">
+        <v>171</v>
+      </c>
+      <c r="K24" s="221"/>
+      <c r="L24" s="222">
+        <v>28</v>
+      </c>
+      <c r="M24" s="223"/>
+      <c r="N24" s="244">
+        <v>6</v>
+      </c>
+      <c r="O24" s="230" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="254">
+      <c r="P24" s="221">
         <v>427</v>
       </c>
-      <c r="E24" s="254">
+      <c r="Q24" s="221">
         <v>323</v>
       </c>
-      <c r="F24" s="28">
+      <c r="R24" s="254">
         <v>66</v>
       </c>
-      <c r="G24" s="61"/>
-      <c r="H24" s="10">
-        <v>6</v>
-      </c>
-      <c r="I24" s="245" t="s">
-        <v>122</v>
-      </c>
-      <c r="J24" s="156">
-        <v>171</v>
-      </c>
-      <c r="K24" s="157"/>
-      <c r="L24" s="22">
-        <v>28</v>
-      </c>
-      <c r="M24" s="61"/>
-      <c r="N24" s="10">
-        <v>6</v>
-      </c>
-      <c r="O24" s="226" t="s">
-        <v>5</v>
-      </c>
-      <c r="P24" s="254">
-        <v>427</v>
-      </c>
-      <c r="Q24" s="254">
-        <v>323</v>
-      </c>
-      <c r="R24" s="25">
-        <v>66</v>
-      </c>
-      <c r="S24" s="61"/>
-      <c r="T24" s="47"/>
-      <c r="U24" s="11"/>
+      <c r="S24" s="223"/>
+      <c r="T24" s="245"/>
+      <c r="U24" s="263"/>
       <c r="V24" s="44"/>
       <c r="W24" s="44"/>
       <c r="X24" s="44"/>
       <c r="Y24"/>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B25" s="261"/>
-      <c r="C25" s="261"/>
-      <c r="D25" s="261"/>
-      <c r="E25" s="261"/>
-      <c r="F25" s="261"/>
-      <c r="G25" s="261"/>
-      <c r="H25" s="261"/>
-      <c r="I25" s="261"/>
-      <c r="J25" s="261"/>
-      <c r="K25" s="261"/>
-      <c r="L25" s="261"/>
-      <c r="M25" s="261"/>
-      <c r="N25" s="261"/>
-      <c r="O25" s="261"/>
-      <c r="P25" s="261"/>
-      <c r="Q25" s="261"/>
-      <c r="R25" s="261"/>
-      <c r="S25" s="261"/>
-      <c r="T25" s="261"/>
-      <c r="U25" s="261"/>
+      <c r="B25" s="247"/>
+      <c r="C25" s="247"/>
+      <c r="D25" s="247"/>
+      <c r="E25" s="247"/>
+      <c r="F25" s="247"/>
+      <c r="G25" s="247"/>
+      <c r="H25" s="247"/>
+      <c r="I25" s="247"/>
+      <c r="J25" s="247"/>
+      <c r="K25" s="247"/>
+      <c r="L25" s="247"/>
+      <c r="M25" s="247"/>
+      <c r="N25" s="247"/>
+      <c r="O25" s="247"/>
+      <c r="P25" s="247"/>
+      <c r="Q25" s="247"/>
+      <c r="R25" s="247"/>
+      <c r="S25" s="247"/>
+      <c r="T25" s="247"/>
+      <c r="U25" s="247"/>
       <c r="V25" s="5"/>
       <c r="W25" s="5"/>
       <c r="X25" s="5"/>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A26" s="259"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="136" t="s">
+      <c r="A26" s="210"/>
+      <c r="B26" s="214"/>
+      <c r="C26" s="214" t="s">
         <v>132</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="214" t="s">
         <v>2</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="214" t="s">
         <v>3</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="214" t="s">
         <v>1</v>
       </c>
-      <c r="G26" s="45"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="109" t="s">
+      <c r="G26" s="218"/>
+      <c r="H26" s="213"/>
+      <c r="I26" s="213" t="s">
         <v>135</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="J26" s="214" t="s">
         <v>2</v>
       </c>
-      <c r="K26" s="2" t="s">
+      <c r="K26" s="214" t="s">
         <v>3</v>
       </c>
-      <c r="L26" s="2" t="s">
+      <c r="L26" s="214" t="s">
         <v>1</v>
       </c>
-      <c r="M26" s="49"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="109" t="s">
+      <c r="M26" s="216"/>
+      <c r="N26" s="213"/>
+      <c r="O26" s="213" t="s">
         <v>136</v>
       </c>
-      <c r="P26" s="2" t="s">
+      <c r="P26" s="214" t="s">
         <v>2</v>
       </c>
-      <c r="Q26" s="2" t="s">
+      <c r="Q26" s="214" t="s">
         <v>3</v>
       </c>
-      <c r="R26" s="2" t="s">
+      <c r="R26" s="214" t="s">
         <v>1</v>
       </c>
-      <c r="S26" s="49"/>
-      <c r="T26" s="49"/>
-      <c r="U26" s="49"/>
+      <c r="S26" s="216"/>
+      <c r="T26" s="216"/>
+      <c r="U26" s="216"/>
       <c r="V26" s="45"/>
       <c r="W26" s="45"/>
       <c r="X26" s="45"/>
     </row>
     <row r="27" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="259"/>
-      <c r="B27" s="98">
+      <c r="A27" s="210"/>
+      <c r="B27" s="219">
         <v>1</v>
       </c>
-      <c r="C27" s="237" t="s">
+      <c r="C27" s="230" t="s">
         <v>115</v>
       </c>
-      <c r="D27" s="156">
+      <c r="D27" s="221">
         <v>483</v>
       </c>
-      <c r="E27" s="157"/>
-      <c r="F27" s="14">
+      <c r="E27" s="221"/>
+      <c r="F27" s="244">
         <v>67</v>
       </c>
-      <c r="G27" s="61"/>
-      <c r="H27" s="28">
+      <c r="G27" s="223"/>
+      <c r="H27" s="224">
         <v>1</v>
       </c>
-      <c r="I27" s="237" t="s">
+      <c r="I27" s="230" t="s">
         <v>13</v>
       </c>
-      <c r="J27" s="156">
+      <c r="J27" s="221">
         <v>397</v>
       </c>
-      <c r="K27" s="157">
+      <c r="K27" s="221">
         <v>165</v>
       </c>
-      <c r="L27" s="28">
+      <c r="L27" s="224">
         <v>61</v>
       </c>
-      <c r="M27" s="61"/>
-      <c r="N27" s="18">
+      <c r="M27" s="223"/>
+      <c r="N27" s="224">
         <v>1</v>
       </c>
-      <c r="O27" s="237" t="s">
+      <c r="O27" s="230" t="s">
         <v>19</v>
       </c>
-      <c r="P27" s="156">
+      <c r="P27" s="221">
         <v>498</v>
       </c>
-      <c r="Q27" s="157">
+      <c r="Q27" s="221">
         <v>309</v>
       </c>
-      <c r="R27" s="21">
+      <c r="R27" s="232">
         <v>58</v>
       </c>
-      <c r="S27" s="61"/>
-      <c r="T27" s="50"/>
-      <c r="U27" s="56"/>
+      <c r="S27" s="223"/>
+      <c r="T27" s="227"/>
+      <c r="U27" s="266"/>
       <c r="V27" s="57"/>
       <c r="W27" s="58"/>
       <c r="X27" s="59"/>
     </row>
     <row r="28" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="259"/>
-      <c r="B28" s="18">
+      <c r="A28" s="210"/>
+      <c r="B28" s="224">
         <v>2</v>
       </c>
-      <c r="C28" s="237" t="s">
+      <c r="C28" s="230" t="s">
         <v>118</v>
       </c>
-      <c r="D28" s="156">
+      <c r="D28" s="221">
         <v>377</v>
       </c>
-      <c r="E28" s="156">
+      <c r="E28" s="221">
         <v>114</v>
       </c>
-      <c r="F28" s="18">
+      <c r="F28" s="224">
         <v>70</v>
       </c>
-      <c r="G28" s="61"/>
-      <c r="H28" s="28">
+      <c r="G28" s="223"/>
+      <c r="H28" s="224">
         <v>2</v>
       </c>
-      <c r="I28" s="238" t="s">
+      <c r="I28" s="220" t="s">
         <v>8</v>
       </c>
-      <c r="J28" s="156">
+      <c r="J28" s="221">
         <v>522</v>
       </c>
-      <c r="K28" s="157">
+      <c r="K28" s="221">
         <v>372</v>
       </c>
-      <c r="L28" s="193">
+      <c r="L28" s="270">
         <v>27</v>
       </c>
-      <c r="M28" s="61"/>
-      <c r="N28" s="18">
+      <c r="M28" s="223"/>
+      <c r="N28" s="224">
         <v>2</v>
       </c>
-      <c r="O28" s="237" t="s">
+      <c r="O28" s="230" t="s">
         <v>65</v>
       </c>
-      <c r="P28" s="157">
+      <c r="P28" s="221">
         <v>262</v>
       </c>
-      <c r="Q28" s="156">
+      <c r="Q28" s="221">
         <v>146</v>
       </c>
-      <c r="R28" s="118">
+      <c r="R28" s="252">
         <v>73</v>
       </c>
-      <c r="S28" s="61"/>
-      <c r="T28" s="50"/>
-      <c r="U28" s="56"/>
+      <c r="S28" s="223"/>
+      <c r="T28" s="227"/>
+      <c r="U28" s="266"/>
       <c r="V28" s="57"/>
       <c r="W28" s="58"/>
       <c r="X28" s="59"/>
     </row>
     <row r="29" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="259"/>
-      <c r="B29" s="19">
+      <c r="A29" s="210"/>
+      <c r="B29" s="222">
         <v>3</v>
       </c>
-      <c r="C29" s="208" t="s">
+      <c r="C29" s="230" t="s">
         <v>124</v>
       </c>
-      <c r="D29" s="157">
+      <c r="D29" s="221">
         <v>452</v>
       </c>
-      <c r="E29" s="156">
+      <c r="E29" s="221">
         <v>136</v>
       </c>
-      <c r="F29" s="21">
+      <c r="F29" s="232">
         <v>77</v>
       </c>
-      <c r="G29" s="61"/>
-      <c r="H29" s="22">
+      <c r="G29" s="223"/>
+      <c r="H29" s="222">
         <v>3</v>
       </c>
-      <c r="I29" s="256" t="s">
+      <c r="I29" s="271" t="s">
         <v>73</v>
       </c>
-      <c r="J29" s="156">
+      <c r="J29" s="221">
         <v>381</v>
       </c>
-      <c r="K29" s="156">
+      <c r="K29" s="221">
         <v>216</v>
       </c>
-      <c r="L29" s="21">
+      <c r="L29" s="232">
         <v>57</v>
       </c>
-      <c r="M29" s="61"/>
-      <c r="N29" s="19">
+      <c r="M29" s="223"/>
+      <c r="N29" s="222">
         <v>3</v>
       </c>
-      <c r="O29" s="226" t="s">
+      <c r="O29" s="230" t="s">
         <v>84</v>
       </c>
-      <c r="P29" s="156">
+      <c r="P29" s="221">
         <v>409</v>
       </c>
-      <c r="Q29" s="157">
+      <c r="Q29" s="221">
         <v>174</v>
       </c>
-      <c r="R29" s="22">
+      <c r="R29" s="222">
         <v>46</v>
       </c>
-      <c r="S29" s="61"/>
-      <c r="T29" s="46"/>
-      <c r="U29" s="56"/>
+      <c r="S29" s="223"/>
+      <c r="T29" s="238"/>
+      <c r="U29" s="266"/>
       <c r="V29" s="57"/>
       <c r="W29" s="58"/>
       <c r="X29" s="59"/>
     </row>
     <row r="30" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="259"/>
-      <c r="B30" s="18">
+      <c r="A30" s="210"/>
+      <c r="B30" s="224">
         <v>4</v>
       </c>
-      <c r="C30" s="238" t="s">
+      <c r="C30" s="220" t="s">
         <v>117</v>
       </c>
-      <c r="D30" s="156">
+      <c r="D30" s="221">
         <v>457</v>
       </c>
-      <c r="E30" s="157">
+      <c r="E30" s="221">
         <v>236</v>
       </c>
-      <c r="F30" s="115">
+      <c r="F30" s="225">
         <v>43</v>
       </c>
-      <c r="G30" s="61"/>
-      <c r="H30" s="28">
+      <c r="G30" s="223"/>
+      <c r="H30" s="224">
         <v>4</v>
       </c>
-      <c r="I30" s="223" t="s">
+      <c r="I30" s="242" t="s">
         <v>107</v>
       </c>
-      <c r="J30" s="218" t="s">
+      <c r="J30" s="248" t="s">
         <v>33</v>
       </c>
-      <c r="K30" s="212" t="s">
+      <c r="K30" s="248" t="s">
         <v>33</v>
       </c>
-      <c r="L30" s="115">
+      <c r="L30" s="225">
         <v>142</v>
       </c>
-      <c r="M30" s="61"/>
-      <c r="N30" s="18">
+      <c r="M30" s="223"/>
+      <c r="N30" s="224">
         <v>4</v>
       </c>
-      <c r="O30" s="234" t="s">
+      <c r="O30" s="240" t="s">
         <v>91</v>
       </c>
-      <c r="P30" s="233" t="s">
+      <c r="P30" s="272" t="s">
         <v>33</v>
       </c>
-      <c r="Q30" s="233" t="s">
+      <c r="Q30" s="272" t="s">
         <v>33</v>
       </c>
-      <c r="R30" s="118">
+      <c r="R30" s="252">
         <v>136</v>
       </c>
-      <c r="S30" s="61"/>
-      <c r="T30" s="50"/>
-      <c r="U30" s="56"/>
+      <c r="S30" s="223"/>
+      <c r="T30" s="227"/>
+      <c r="U30" s="266"/>
       <c r="V30" s="57"/>
       <c r="W30" s="58"/>
       <c r="X30" s="59"/>
     </row>
     <row r="31" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="259"/>
-      <c r="B31" s="19">
+      <c r="A31" s="210"/>
+      <c r="B31" s="222">
         <v>5</v>
       </c>
-      <c r="C31" s="237" t="s">
+      <c r="C31" s="230" t="s">
         <v>114</v>
       </c>
-      <c r="D31" s="156">
+      <c r="D31" s="221">
         <v>214</v>
       </c>
-      <c r="E31" s="157"/>
-      <c r="F31" s="25">
+      <c r="E31" s="221"/>
+      <c r="F31" s="254">
         <v>45</v>
       </c>
-      <c r="G31" s="61"/>
-      <c r="H31" s="198">
+      <c r="G31" s="223"/>
+      <c r="H31" s="269">
         <v>5</v>
       </c>
-      <c r="I31" s="224" t="s">
+      <c r="I31" s="240" t="s">
         <v>108</v>
       </c>
-      <c r="J31" s="250">
+      <c r="J31" s="221">
         <v>118</v>
       </c>
-      <c r="K31" s="245"/>
-      <c r="L31" s="198">
+      <c r="K31" s="220"/>
+      <c r="L31" s="269">
         <v>131</v>
       </c>
-      <c r="M31" s="61"/>
-      <c r="N31" s="19">
+      <c r="M31" s="223"/>
+      <c r="N31" s="222">
         <v>5</v>
       </c>
-      <c r="O31" s="234" t="s">
+      <c r="O31" s="240" t="s">
         <v>48</v>
       </c>
-      <c r="P31" s="233" t="s">
+      <c r="P31" s="272" t="s">
         <v>33</v>
       </c>
-      <c r="Q31" s="233" t="s">
+      <c r="Q31" s="272" t="s">
         <v>33</v>
       </c>
-      <c r="R31" s="28">
+      <c r="R31" s="224">
         <v>116</v>
       </c>
-      <c r="S31" s="61"/>
-      <c r="T31" s="46"/>
-      <c r="U31" s="56"/>
+      <c r="S31" s="223"/>
+      <c r="T31" s="238"/>
+      <c r="U31" s="266"/>
       <c r="V31" s="57"/>
       <c r="W31" s="58"/>
       <c r="X31" s="59"/>
     </row>
     <row r="32" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="259"/>
-      <c r="B32" s="10">
+      <c r="A32" s="210"/>
+      <c r="B32" s="244">
         <v>6</v>
       </c>
-      <c r="C32" s="226" t="s">
+      <c r="C32" s="230" t="s">
         <v>83</v>
       </c>
-      <c r="D32" s="157">
+      <c r="D32" s="221">
         <v>143</v>
       </c>
-      <c r="E32" s="156">
+      <c r="E32" s="221">
         <v>24</v>
       </c>
-      <c r="F32" s="34">
+      <c r="F32" s="229">
         <v>50</v>
       </c>
-      <c r="G32" s="61"/>
-      <c r="H32" s="14">
+      <c r="G32" s="223"/>
+      <c r="H32" s="244">
         <v>6</v>
       </c>
-      <c r="I32" s="192" t="s">
+      <c r="I32" s="220" t="s">
         <v>27</v>
       </c>
-      <c r="J32" s="157">
+      <c r="J32" s="221">
         <v>458</v>
       </c>
-      <c r="K32" s="156">
+      <c r="K32" s="221">
         <v>43</v>
       </c>
-      <c r="L32" s="14">
+      <c r="L32" s="244">
         <v>80</v>
       </c>
-      <c r="M32" s="71"/>
-      <c r="N32" s="10">
+      <c r="M32" s="262"/>
+      <c r="N32" s="244">
         <v>6</v>
       </c>
-      <c r="O32" s="238" t="s">
+      <c r="O32" s="220" t="s">
         <v>119</v>
       </c>
-      <c r="P32" s="156">
+      <c r="P32" s="221">
         <v>322</v>
       </c>
-      <c r="Q32" s="157">
+      <c r="Q32" s="221">
         <v>149</v>
       </c>
-      <c r="R32" s="14">
+      <c r="R32" s="244">
         <v>81</v>
       </c>
-      <c r="S32" s="61"/>
-      <c r="T32" s="47"/>
-      <c r="U32" s="56"/>
+      <c r="S32" s="223"/>
+      <c r="T32" s="245"/>
+      <c r="U32" s="266"/>
       <c r="V32" s="57"/>
       <c r="W32" s="58"/>
       <c r="X32" s="59"/>
     </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B33" s="243"/>
+      <c r="C33" s="243"/>
+      <c r="D33" s="243"/>
+      <c r="E33" s="243"/>
+      <c r="F33" s="243"/>
+      <c r="G33" s="243"/>
+      <c r="H33" s="243"/>
+      <c r="I33" s="243"/>
+      <c r="J33" s="243"/>
+      <c r="K33" s="243"/>
+      <c r="L33" s="243"/>
+      <c r="M33" s="243"/>
+      <c r="N33" s="243"/>
+      <c r="O33" s="243"/>
+      <c r="P33" s="243"/>
+      <c r="Q33" s="243"/>
+      <c r="R33" s="243"/>
+      <c r="S33" s="243"/>
+      <c r="T33" s="243"/>
+      <c r="U33" s="243"/>
+    </row>
     <row r="34" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="260"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="136" t="s">
+      <c r="A34" s="211"/>
+      <c r="B34" s="214"/>
+      <c r="C34" s="214" t="s">
         <v>101</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="214" t="s">
         <v>2</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="214" t="s">
         <v>3</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" s="214" t="s">
         <v>1</v>
       </c>
-      <c r="G34" s="49"/>
-      <c r="H34" s="194"/>
-      <c r="I34" s="109"/>
-      <c r="J34" s="2" t="s">
+      <c r="G34" s="216"/>
+      <c r="H34" s="213"/>
+      <c r="I34" s="213"/>
+      <c r="J34" s="214" t="s">
         <v>2</v>
       </c>
-      <c r="K34" s="2" t="s">
+      <c r="K34" s="214" t="s">
         <v>3</v>
       </c>
-      <c r="L34" s="2" t="s">
+      <c r="L34" s="214" t="s">
         <v>1</v>
       </c>
-      <c r="N34" s="4"/>
-      <c r="O34" s="109"/>
-      <c r="P34" s="2" t="s">
+      <c r="M34" s="243"/>
+      <c r="N34" s="213"/>
+      <c r="O34" s="213"/>
+      <c r="P34" s="214" t="s">
         <v>2</v>
       </c>
-      <c r="Q34" s="2" t="s">
+      <c r="Q34" s="214" t="s">
         <v>3</v>
       </c>
-      <c r="R34" s="2" t="s">
+      <c r="R34" s="214" t="s">
         <v>1</v>
       </c>
-      <c r="T34" s="55"/>
-      <c r="U34" s="56"/>
+      <c r="S34" s="243"/>
+      <c r="T34" s="273"/>
+      <c r="U34" s="266"/>
       <c r="V34" s="57"/>
       <c r="W34" s="58"/>
       <c r="X34" s="59"/>
     </row>
     <row r="35" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="260"/>
-      <c r="B35" s="98">
+      <c r="A35" s="211"/>
+      <c r="B35" s="219">
         <v>1</v>
       </c>
-      <c r="C35" s="237" t="s">
+      <c r="C35" s="230" t="s">
         <v>12</v>
       </c>
-      <c r="D35" s="157">
+      <c r="D35" s="221">
         <v>384</v>
       </c>
-      <c r="E35" s="156">
+      <c r="E35" s="221">
         <v>246</v>
       </c>
-      <c r="F35" s="113">
+      <c r="F35" s="225">
         <v>54</v>
       </c>
-      <c r="G35" s="61"/>
-      <c r="H35" s="204">
+      <c r="G35" s="223"/>
+      <c r="H35" s="274">
         <v>1</v>
       </c>
-      <c r="I35" s="226"/>
-      <c r="J35" s="222"/>
-      <c r="K35" s="210"/>
-      <c r="L35" s="22"/>
-      <c r="N35" s="116">
+      <c r="I35" s="230"/>
+      <c r="J35" s="251"/>
+      <c r="K35" s="251"/>
+      <c r="L35" s="222"/>
+      <c r="M35" s="243"/>
+      <c r="N35" s="275">
         <v>1</v>
       </c>
-      <c r="O35" s="226"/>
-      <c r="P35" s="210"/>
-      <c r="Q35" s="222"/>
-      <c r="R35" s="99"/>
-      <c r="T35" s="12"/>
-      <c r="U35" s="12"/>
+      <c r="O35" s="230"/>
+      <c r="P35" s="251"/>
+      <c r="Q35" s="251"/>
+      <c r="R35" s="249"/>
+      <c r="S35" s="243"/>
+      <c r="T35" s="243"/>
+      <c r="U35" s="243"/>
       <c r="V35" s="12"/>
       <c r="W35" s="12"/>
       <c r="X35" s="12"/>
     </row>
     <row r="36" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="260"/>
-      <c r="B36" s="18">
+      <c r="A36" s="211"/>
+      <c r="B36" s="224">
         <v>2</v>
       </c>
-      <c r="C36" s="208"/>
-      <c r="D36" s="212"/>
-      <c r="E36" s="218"/>
-      <c r="F36" s="115"/>
-      <c r="G36" s="61"/>
-      <c r="H36" s="28">
+      <c r="C36" s="205" t="s">
+        <v>141</v>
+      </c>
+      <c r="D36" s="248"/>
+      <c r="E36" s="248"/>
+      <c r="F36" s="225"/>
+      <c r="G36" s="223"/>
+      <c r="H36" s="224">
         <v>2</v>
       </c>
-      <c r="I36" s="232"/>
-      <c r="J36" s="226"/>
-      <c r="K36" s="226"/>
-      <c r="L36" s="14"/>
-      <c r="N36" s="28">
+      <c r="I36" s="240"/>
+      <c r="J36" s="230"/>
+      <c r="K36" s="230"/>
+      <c r="L36" s="244"/>
+      <c r="M36" s="243"/>
+      <c r="N36" s="224">
         <v>2</v>
       </c>
-      <c r="O36" s="226"/>
-      <c r="P36" s="157"/>
-      <c r="Q36" s="156"/>
-      <c r="R36" s="118"/>
-      <c r="T36" s="12"/>
-      <c r="U36" s="12"/>
+      <c r="O36" s="230"/>
+      <c r="P36" s="221"/>
+      <c r="Q36" s="221"/>
+      <c r="R36" s="252"/>
+      <c r="S36" s="243"/>
+      <c r="T36" s="243"/>
+      <c r="U36" s="243"/>
       <c r="V36" s="12"/>
       <c r="W36" s="12"/>
       <c r="X36" s="12"/>
     </row>
     <row r="37" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="260"/>
-      <c r="B37" s="19">
+      <c r="A37" s="211"/>
+      <c r="B37" s="222">
         <v>3</v>
       </c>
-      <c r="C37" s="237" t="s">
-        <v>118</v>
-      </c>
-      <c r="D37" s="156">
+      <c r="C37" s="230" t="s">
+        <v>142</v>
+      </c>
+      <c r="D37" s="221">
         <v>377</v>
       </c>
-      <c r="E37" s="156">
+      <c r="E37" s="221">
         <v>114</v>
       </c>
-      <c r="F37" s="113">
+      <c r="F37" s="225">
         <v>70</v>
       </c>
-      <c r="G37" s="61"/>
-      <c r="H37" s="22">
+      <c r="G37" s="223"/>
+      <c r="H37" s="222">
         <v>3</v>
       </c>
-      <c r="I37" s="227"/>
-      <c r="J37" s="210"/>
-      <c r="K37" s="222"/>
-      <c r="L37" s="21"/>
-      <c r="N37" s="22">
+      <c r="I37" s="261"/>
+      <c r="J37" s="251"/>
+      <c r="K37" s="251"/>
+      <c r="L37" s="232"/>
+      <c r="M37" s="243"/>
+      <c r="N37" s="222">
         <v>3</v>
       </c>
-      <c r="O37" s="237"/>
-      <c r="P37" s="222"/>
-      <c r="Q37" s="210"/>
-      <c r="R37" s="115"/>
-      <c r="T37" s="12"/>
-      <c r="U37" s="12"/>
+      <c r="O37" s="230"/>
+      <c r="P37" s="251"/>
+      <c r="Q37" s="251"/>
+      <c r="R37" s="225"/>
+      <c r="S37" s="243"/>
+      <c r="T37" s="243"/>
+      <c r="U37" s="243"/>
       <c r="V37" s="12"/>
       <c r="W37" s="12"/>
       <c r="X37" s="12"/>
     </row>
     <row r="38" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="260"/>
-      <c r="B38" s="18">
+      <c r="A38" s="211"/>
+      <c r="B38" s="224">
         <v>4</v>
       </c>
-      <c r="C38" s="238" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" s="156">
+      <c r="C38" s="220" t="s">
+        <v>143</v>
+      </c>
+      <c r="D38" s="221">
         <v>522</v>
       </c>
-      <c r="E38" s="157">
+      <c r="E38" s="221">
         <v>372</v>
       </c>
-      <c r="F38" s="113">
+      <c r="F38" s="225">
         <v>27</v>
       </c>
-      <c r="G38" s="61"/>
-      <c r="H38" s="28">
+      <c r="G38" s="223"/>
+      <c r="H38" s="224">
         <v>4</v>
       </c>
-      <c r="I38" s="234"/>
-      <c r="J38" s="250"/>
-      <c r="K38" s="245"/>
-      <c r="L38" s="28"/>
-      <c r="N38" s="28">
+      <c r="I38" s="240"/>
+      <c r="J38" s="221"/>
+      <c r="K38" s="220"/>
+      <c r="L38" s="224"/>
+      <c r="M38" s="243"/>
+      <c r="N38" s="224">
         <v>4</v>
       </c>
-      <c r="O38" s="158"/>
-      <c r="P38" s="157"/>
-      <c r="Q38" s="156"/>
-      <c r="R38" s="113"/>
-      <c r="T38" s="12"/>
-      <c r="U38" s="12"/>
+      <c r="O38" s="220"/>
+      <c r="P38" s="221"/>
+      <c r="Q38" s="221"/>
+      <c r="R38" s="225"/>
+      <c r="S38" s="243"/>
+      <c r="T38" s="243"/>
+      <c r="U38" s="243"/>
       <c r="V38" s="12"/>
       <c r="W38" s="12"/>
       <c r="X38" s="12"/>
     </row>
     <row r="39" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="260"/>
-      <c r="B39" s="19">
+      <c r="A39" s="211"/>
+      <c r="B39" s="222">
         <v>5</v>
       </c>
-      <c r="C39" s="255" t="s">
+      <c r="C39" s="220" t="s">
         <v>61</v>
       </c>
-      <c r="D39" s="156">
+      <c r="D39" s="221">
         <v>359</v>
       </c>
-      <c r="E39" s="157">
+      <c r="E39" s="221">
         <v>90</v>
       </c>
-      <c r="F39" s="113">
+      <c r="F39" s="225">
         <v>36</v>
       </c>
-      <c r="G39" s="61"/>
-      <c r="H39" s="22">
+      <c r="G39" s="223"/>
+      <c r="H39" s="222">
         <v>5</v>
       </c>
-      <c r="I39" s="155"/>
-      <c r="J39" s="157"/>
-      <c r="K39" s="156"/>
-      <c r="L39" s="34"/>
-      <c r="N39" s="22">
+      <c r="I39" s="220"/>
+      <c r="J39" s="221"/>
+      <c r="K39" s="221"/>
+      <c r="L39" s="229"/>
+      <c r="M39" s="243"/>
+      <c r="N39" s="222">
         <v>5</v>
       </c>
-      <c r="O39" s="234"/>
-      <c r="P39" s="235"/>
-      <c r="Q39" s="236"/>
-      <c r="R39" s="34"/>
-      <c r="T39" s="12"/>
-      <c r="U39" s="12"/>
+      <c r="O39" s="240"/>
+      <c r="P39" s="251"/>
+      <c r="Q39" s="261"/>
+      <c r="R39" s="229"/>
+      <c r="S39" s="243"/>
+      <c r="T39" s="243"/>
+      <c r="U39" s="243"/>
       <c r="V39" s="12"/>
       <c r="W39" s="12"/>
       <c r="X39" s="12"/>
     </row>
     <row r="40" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="260"/>
-      <c r="B40" s="10">
+      <c r="A40" s="211"/>
+      <c r="B40" s="244">
         <v>6</v>
       </c>
-      <c r="C40" s="192" t="s">
+      <c r="C40" s="220" t="s">
         <v>120</v>
       </c>
-      <c r="D40" s="156">
+      <c r="D40" s="221">
         <v>144</v>
       </c>
-      <c r="E40" s="156">
+      <c r="E40" s="221">
         <v>27</v>
       </c>
-      <c r="F40" s="21">
+      <c r="F40" s="232">
         <v>87</v>
       </c>
-      <c r="G40" s="61"/>
-      <c r="H40" s="14">
+      <c r="G40" s="223"/>
+      <c r="H40" s="244">
         <v>6</v>
       </c>
-      <c r="I40" s="159"/>
-      <c r="J40" s="157"/>
-      <c r="K40" s="156"/>
-      <c r="L40" s="28"/>
-      <c r="N40" s="14">
+      <c r="I40" s="220"/>
+      <c r="J40" s="221"/>
+      <c r="K40" s="221"/>
+      <c r="L40" s="224"/>
+      <c r="M40" s="243"/>
+      <c r="N40" s="244">
         <v>6</v>
       </c>
-      <c r="O40" s="238"/>
-      <c r="P40" s="156"/>
-      <c r="Q40" s="156"/>
-      <c r="R40" s="207"/>
-      <c r="T40" s="12"/>
-      <c r="U40" s="12"/>
+      <c r="O40" s="220"/>
+      <c r="P40" s="221"/>
+      <c r="Q40" s="221"/>
+      <c r="R40" s="244"/>
+      <c r="S40" s="243"/>
+      <c r="T40" s="243"/>
+      <c r="U40" s="243"/>
       <c r="V40" s="12"/>
       <c r="W40" s="12"/>
       <c r="X40" s="12"/>
@@ -4182,14 +4258,14 @@
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
       <c r="B42" s="2"/>
-      <c r="C42" s="201"/>
-      <c r="D42" s="202" t="s">
+      <c r="C42" s="195"/>
+      <c r="D42" s="196" t="s">
         <v>2</v>
       </c>
-      <c r="E42" s="202" t="s">
+      <c r="E42" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="202" t="s">
+      <c r="F42" s="196" t="s">
         <v>1</v>
       </c>
       <c r="H42" s="49"/>
@@ -4210,12 +4286,12 @@
     </row>
     <row r="43" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
-      <c r="B43" s="199">
+      <c r="B43" s="193">
         <v>1</v>
       </c>
-      <c r="C43" s="205"/>
-      <c r="D43" s="214"/>
-      <c r="E43" s="214"/>
+      <c r="C43" s="197"/>
+      <c r="D43" s="201"/>
+      <c r="E43" s="201"/>
       <c r="F43" s="22"/>
       <c r="H43" s="50"/>
       <c r="I43" s="76"/>
@@ -4235,12 +4311,12 @@
     </row>
     <row r="44" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
-      <c r="B44" s="196">
+      <c r="B44" s="192">
         <v>2</v>
       </c>
-      <c r="C44" s="209"/>
-      <c r="D44" s="192"/>
-      <c r="E44" s="192"/>
+      <c r="C44" s="200"/>
+      <c r="D44" s="190"/>
+      <c r="E44" s="190"/>
       <c r="F44" s="14"/>
       <c r="H44" s="50"/>
       <c r="I44" s="81"/>
@@ -4260,12 +4336,12 @@
     </row>
     <row r="45" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
-      <c r="B45" s="195">
+      <c r="B45" s="191">
         <v>3</v>
       </c>
-      <c r="C45" s="209"/>
-      <c r="D45" s="208"/>
-      <c r="E45" s="208"/>
+      <c r="C45" s="200"/>
+      <c r="D45" s="199"/>
+      <c r="E45" s="199"/>
       <c r="F45" s="14"/>
       <c r="H45" s="46"/>
       <c r="I45" s="76"/>
@@ -4285,12 +4361,12 @@
     </row>
     <row r="46" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
-      <c r="B46" s="196">
+      <c r="B46" s="192">
         <v>4</v>
       </c>
-      <c r="C46" s="215"/>
-      <c r="D46" s="216"/>
-      <c r="E46" s="217"/>
+      <c r="C46" s="202"/>
+      <c r="D46" s="203"/>
+      <c r="E46" s="204"/>
       <c r="F46" s="99"/>
       <c r="H46" s="86"/>
       <c r="I46" s="56"/>
@@ -4310,12 +4386,12 @@
     </row>
     <row r="47" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
-      <c r="B47" s="195">
+      <c r="B47" s="191">
         <v>5</v>
       </c>
-      <c r="C47" s="206"/>
-      <c r="D47" s="157"/>
-      <c r="E47" s="156"/>
+      <c r="C47" s="198"/>
+      <c r="D47" s="156"/>
+      <c r="E47" s="155"/>
       <c r="F47" s="34"/>
       <c r="H47" s="46"/>
       <c r="I47" s="76"/>
@@ -4335,12 +4411,12 @@
     </row>
     <row r="48" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
-      <c r="B48" s="200">
+      <c r="B48" s="194">
         <v>6</v>
       </c>
-      <c r="C48" s="192"/>
-      <c r="D48" s="191"/>
-      <c r="E48" s="156"/>
+      <c r="C48" s="190"/>
+      <c r="D48" s="189"/>
+      <c r="E48" s="155"/>
       <c r="F48" s="34"/>
       <c r="H48" s="47"/>
       <c r="I48" s="87"/>
@@ -4408,68 +4484,68 @@
       </c>
     </row>
     <row r="5" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C5" s="174">
+      <c r="C5" s="172">
         <v>1</v>
       </c>
-      <c r="D5" s="166" t="s">
+      <c r="D5" s="164" t="s">
         <v>77</v>
       </c>
-      <c r="E5" s="167">
+      <c r="E5" s="165">
         <v>1</v>
       </c>
-      <c r="F5" s="168">
+      <c r="F5" s="166">
         <v>18</v>
       </c>
       <c r="G5" s="22">
         <v>117</v>
       </c>
-      <c r="H5" s="190"/>
+      <c r="H5" s="188"/>
     </row>
     <row r="6" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C6" s="175">
+      <c r="C6" s="173">
         <v>2</v>
       </c>
       <c r="D6" s="154" t="s">
         <v>89</v>
       </c>
-      <c r="E6" s="169">
+      <c r="E6" s="167">
         <v>127</v>
       </c>
-      <c r="F6" s="170"/>
+      <c r="F6" s="168"/>
       <c r="G6" s="34">
         <v>124</v>
       </c>
-      <c r="H6" s="190"/>
+      <c r="H6" s="188"/>
     </row>
     <row r="7" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C7" s="174">
+      <c r="C7" s="172">
         <v>3</v>
       </c>
-      <c r="D7" s="165" t="s">
+      <c r="D7" s="163" t="s">
         <v>80</v>
       </c>
-      <c r="E7" s="164">
+      <c r="E7" s="162">
         <v>356</v>
       </c>
-      <c r="F7" s="162">
+      <c r="F7" s="160">
         <v>285</v>
       </c>
       <c r="G7" s="28">
         <v>11</v>
       </c>
-      <c r="H7" s="190"/>
+      <c r="H7" s="188"/>
     </row>
     <row r="8" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C8" s="26">
         <v>4</v>
       </c>
-      <c r="D8" s="163" t="s">
+      <c r="D8" s="161" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="164">
+      <c r="E8" s="162">
         <v>518</v>
       </c>
-      <c r="F8" s="162">
+      <c r="F8" s="160">
         <v>95</v>
       </c>
       <c r="G8" s="22">
@@ -4477,94 +4553,94 @@
       </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="174">
+      <c r="C9" s="172">
         <v>5</v>
       </c>
-      <c r="D9" s="171" t="s">
+      <c r="D9" s="169" t="s">
         <v>95</v>
       </c>
-      <c r="E9" s="172"/>
-      <c r="F9" s="173"/>
-      <c r="G9" s="172">
+      <c r="E9" s="170"/>
+      <c r="F9" s="171"/>
+      <c r="G9" s="170">
         <v>135</v>
       </c>
-      <c r="H9" s="190">
+      <c r="H9" s="188">
         <v>136</v>
       </c>
     </row>
     <row r="10" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C10" s="175">
+      <c r="C10" s="173">
         <v>6</v>
       </c>
-      <c r="D10" s="161" t="s">
+      <c r="D10" s="159" t="s">
         <v>93</v>
       </c>
-      <c r="E10" s="157">
+      <c r="E10" s="156">
         <v>98</v>
       </c>
-      <c r="F10" s="156">
+      <c r="F10" s="155">
         <v>56</v>
       </c>
       <c r="G10" s="28">
         <v>65</v>
       </c>
-      <c r="H10" s="190"/>
+      <c r="H10" s="188"/>
     </row>
     <row r="11" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C11" s="174">
+      <c r="C11" s="172">
         <v>7</v>
       </c>
-      <c r="D11" s="160" t="s">
+      <c r="D11" s="158" t="s">
         <v>96</v>
       </c>
-      <c r="E11" s="157"/>
-      <c r="F11" s="156"/>
+      <c r="E11" s="156"/>
+      <c r="F11" s="155"/>
       <c r="G11" s="21">
         <v>137</v>
       </c>
-      <c r="H11" s="190"/>
+      <c r="H11" s="188"/>
     </row>
     <row r="12" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C12" s="175">
+      <c r="C12" s="173">
         <v>8</v>
       </c>
-      <c r="D12" s="158" t="s">
+      <c r="D12" s="157" t="s">
         <v>92</v>
       </c>
-      <c r="E12" s="156">
+      <c r="E12" s="155">
         <v>53</v>
       </c>
-      <c r="F12" s="157"/>
+      <c r="F12" s="156"/>
       <c r="G12" s="22">
         <v>125</v>
       </c>
     </row>
     <row r="13" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C13" s="176">
+      <c r="C13" s="174">
         <v>9</v>
       </c>
-      <c r="D13" s="177" t="s">
+      <c r="D13" s="175" t="s">
         <v>90</v>
       </c>
-      <c r="E13" s="178">
+      <c r="E13" s="176">
         <v>230</v>
       </c>
-      <c r="F13" s="179"/>
+      <c r="F13" s="177"/>
       <c r="G13" s="118">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C14" s="174">
+      <c r="C14" s="172">
         <v>10</v>
       </c>
-      <c r="D14" s="180" t="s">
+      <c r="D14" s="178" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="181">
+      <c r="E14" s="179">
         <v>498</v>
       </c>
-      <c r="F14" s="182">
+      <c r="F14" s="180">
         <v>309</v>
       </c>
       <c r="G14" s="22">
@@ -4572,29 +4648,29 @@
       </c>
     </row>
     <row r="15" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C15" s="175">
+      <c r="C15" s="173">
         <v>11</v>
       </c>
-      <c r="D15" s="183" t="s">
+      <c r="D15" s="181" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="181">
+      <c r="E15" s="179">
         <v>100</v>
       </c>
-      <c r="F15" s="182"/>
+      <c r="F15" s="180"/>
       <c r="G15" s="22">
         <v>103</v>
       </c>
     </row>
     <row r="16" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C16" s="174">
+      <c r="C16" s="172">
         <v>12</v>
       </c>
-      <c r="D16" s="184" t="s">
+      <c r="D16" s="182" t="s">
         <v>97</v>
       </c>
-      <c r="E16" s="182"/>
-      <c r="F16" s="181">
+      <c r="E16" s="180"/>
+      <c r="F16" s="179">
         <v>243</v>
       </c>
       <c r="G16" s="25">
@@ -4605,13 +4681,13 @@
       <c r="C17" s="26">
         <v>13</v>
       </c>
-      <c r="D17" s="185" t="s">
+      <c r="D17" s="183" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="182">
+      <c r="E17" s="180">
         <v>142</v>
       </c>
-      <c r="F17" s="186">
+      <c r="F17" s="184">
         <v>45</v>
       </c>
       <c r="G17" s="21">
@@ -4619,16 +4695,16 @@
       </c>
     </row>
     <row r="18" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C18" s="174">
+      <c r="C18" s="172">
         <v>14</v>
       </c>
-      <c r="D18" s="187" t="s">
+      <c r="D18" s="185" t="s">
         <v>55</v>
       </c>
-      <c r="E18" s="181">
+      <c r="E18" s="179">
         <v>442</v>
       </c>
-      <c r="F18" s="188">
+      <c r="F18" s="186">
         <v>112</v>
       </c>
       <c r="G18" s="25">
@@ -4636,16 +4712,16 @@
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="175">
+      <c r="C19" s="173">
         <v>15</v>
       </c>
-      <c r="D19" s="185" t="s">
+      <c r="D19" s="183" t="s">
         <v>91</v>
       </c>
-      <c r="E19" s="189" t="s">
+      <c r="E19" s="187" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="189" t="s">
+      <c r="F19" s="187" t="s">
         <v>33</v>
       </c>
       <c r="G19" s="22">
@@ -4653,7 +4729,7 @@
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="174">
+      <c r="C20" s="172">
         <v>16</v>
       </c>
       <c r="D20" s="153" t="s">
@@ -4679,31 +4755,31 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="257" t="s">
+      <c r="B1" s="208" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="258"/>
-      <c r="D1" s="258"/>
-      <c r="E1" s="258"/>
-      <c r="F1" s="258"/>
-      <c r="G1" s="258"/>
-      <c r="H1" s="258"/>
-      <c r="I1" s="258"/>
-      <c r="J1" s="258"/>
-      <c r="K1" s="258"/>
-      <c r="L1" s="258"/>
-      <c r="M1" s="258"/>
-      <c r="N1" s="258"/>
-      <c r="O1" s="258"/>
-      <c r="P1" s="258"/>
-      <c r="Q1" s="258"/>
-      <c r="R1" s="258"/>
-      <c r="S1" s="258"/>
-      <c r="T1" s="258"/>
-      <c r="U1" s="258"/>
-      <c r="V1" s="258"/>
-      <c r="W1" s="258"/>
-      <c r="X1" s="258"/>
+      <c r="C1" s="209"/>
+      <c r="D1" s="209"/>
+      <c r="E1" s="209"/>
+      <c r="F1" s="209"/>
+      <c r="G1" s="209"/>
+      <c r="H1" s="209"/>
+      <c r="I1" s="209"/>
+      <c r="J1" s="209"/>
+      <c r="K1" s="209"/>
+      <c r="L1" s="209"/>
+      <c r="M1" s="209"/>
+      <c r="N1" s="209"/>
+      <c r="O1" s="209"/>
+      <c r="P1" s="209"/>
+      <c r="Q1" s="209"/>
+      <c r="R1" s="209"/>
+      <c r="S1" s="209"/>
+      <c r="T1" s="209"/>
+      <c r="U1" s="209"/>
+      <c r="V1" s="209"/>
+      <c r="W1" s="209"/>
+      <c r="X1" s="209"/>
       <c r="Y1" s="124"/>
       <c r="Z1" s="124"/>
       <c r="AA1" s="124"/>
@@ -5075,32 +5151,32 @@
       <c r="AA8" s="83"/>
     </row>
     <row r="9" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B9" s="261"/>
-      <c r="C9" s="261"/>
-      <c r="D9" s="261"/>
-      <c r="E9" s="261"/>
-      <c r="F9" s="261"/>
-      <c r="G9" s="261"/>
-      <c r="H9" s="261"/>
-      <c r="I9" s="261"/>
-      <c r="J9" s="261"/>
-      <c r="K9" s="261"/>
-      <c r="L9" s="261"/>
-      <c r="M9" s="261"/>
-      <c r="N9" s="261"/>
-      <c r="O9" s="261"/>
-      <c r="P9" s="261"/>
-      <c r="Q9" s="261"/>
-      <c r="R9" s="261"/>
-      <c r="S9" s="261"/>
-      <c r="T9" s="261"/>
-      <c r="U9" s="261"/>
-      <c r="V9" s="261"/>
-      <c r="W9" s="261"/>
-      <c r="X9" s="261"/>
-      <c r="Y9" s="261"/>
-      <c r="Z9" s="261"/>
-      <c r="AA9" s="261"/>
+      <c r="B9" s="212"/>
+      <c r="C9" s="212"/>
+      <c r="D9" s="212"/>
+      <c r="E9" s="212"/>
+      <c r="F9" s="212"/>
+      <c r="G9" s="212"/>
+      <c r="H9" s="212"/>
+      <c r="I9" s="212"/>
+      <c r="J9" s="212"/>
+      <c r="K9" s="212"/>
+      <c r="L9" s="212"/>
+      <c r="M9" s="212"/>
+      <c r="N9" s="212"/>
+      <c r="O9" s="212"/>
+      <c r="P9" s="212"/>
+      <c r="Q9" s="212"/>
+      <c r="R9" s="212"/>
+      <c r="S9" s="212"/>
+      <c r="T9" s="212"/>
+      <c r="U9" s="212"/>
+      <c r="V9" s="212"/>
+      <c r="W9" s="212"/>
+      <c r="X9" s="212"/>
+      <c r="Y9" s="212"/>
+      <c r="Z9" s="212"/>
+      <c r="AA9" s="212"/>
     </row>
     <row r="10" spans="2:27" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
@@ -5859,32 +5935,32 @@
       <c r="AA24" s="11"/>
     </row>
     <row r="25" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B25" s="261"/>
-      <c r="C25" s="261"/>
-      <c r="D25" s="261"/>
-      <c r="E25" s="261"/>
-      <c r="F25" s="261"/>
-      <c r="G25" s="261"/>
-      <c r="H25" s="261"/>
-      <c r="I25" s="261"/>
-      <c r="J25" s="261"/>
-      <c r="K25" s="261"/>
-      <c r="L25" s="261"/>
-      <c r="M25" s="261"/>
-      <c r="N25" s="261"/>
-      <c r="O25" s="261"/>
-      <c r="P25" s="261"/>
-      <c r="Q25" s="261"/>
-      <c r="R25" s="261"/>
-      <c r="S25" s="261"/>
-      <c r="T25" s="261"/>
-      <c r="U25" s="261"/>
-      <c r="V25" s="261"/>
-      <c r="W25" s="261"/>
-      <c r="X25" s="261"/>
-      <c r="Y25" s="261"/>
-      <c r="Z25" s="261"/>
-      <c r="AA25" s="261"/>
+      <c r="B25" s="212"/>
+      <c r="C25" s="212"/>
+      <c r="D25" s="212"/>
+      <c r="E25" s="212"/>
+      <c r="F25" s="212"/>
+      <c r="G25" s="212"/>
+      <c r="H25" s="212"/>
+      <c r="I25" s="212"/>
+      <c r="J25" s="212"/>
+      <c r="K25" s="212"/>
+      <c r="L25" s="212"/>
+      <c r="M25" s="212"/>
+      <c r="N25" s="212"/>
+      <c r="O25" s="212"/>
+      <c r="P25" s="212"/>
+      <c r="Q25" s="212"/>
+      <c r="R25" s="212"/>
+      <c r="S25" s="212"/>
+      <c r="T25" s="212"/>
+      <c r="U25" s="212"/>
+      <c r="V25" s="212"/>
+      <c r="W25" s="212"/>
+      <c r="X25" s="212"/>
+      <c r="Y25" s="212"/>
+      <c r="Z25" s="212"/>
+      <c r="AA25" s="212"/>
     </row>
     <row r="26" spans="2:27" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>

</xml_diff>